<commit_message>
Update input processing script and example data
</commit_message>
<xml_diff>
--- a/scripts/processing/output/SBDI-ASV-1-adm.xlsx
+++ b/scripts/processing/output/SBDI-ASV-1-adm.xlsx
@@ -1,1175 +1,1165 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maria.prager/code/github/mol-mod/scripts/processing/output/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BE2C2D-D75C-DB4A-9BBB-C84B873423F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="500" windowWidth="13120" windowHeight="6100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="dataset" sheetId="1" r:id="rId1"/>
-    <sheet name="event" sheetId="2" r:id="rId2"/>
-    <sheet name="mixs" sheetId="3" r:id="rId3"/>
-    <sheet name="emof" sheetId="4" r:id="rId4"/>
-    <sheet name="asv" sheetId="5" r:id="rId5"/>
-    <sheet name="occurrence" sheetId="6" r:id="rId6"/>
-    <sheet name="annotation" sheetId="7" r:id="rId7"/>
+    <sheet name="dataset" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="event" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="mixs" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="emof" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="asv" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="occurrence" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="annotation" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="378">
-  <si>
-    <t>datasetID</t>
-  </si>
-  <si>
-    <t>datasetName</t>
-  </si>
-  <si>
-    <t>filename</t>
-  </si>
-  <si>
-    <t>bioatlas_resource_uid</t>
-  </si>
-  <si>
-    <t>ipt_resource_id</t>
-  </si>
-  <si>
-    <t>SBDI-ASV-1</t>
-  </si>
-  <si>
-    <t>16S data from: Diversity of Pico- to Mesoplankton along the 2000 km Salinity Gradient of the Baltic Sea (Hu et al. 2016)</t>
-  </si>
-  <si>
-    <t>jane.doe@univ.se_210902-212121_ampliseq.xlsx</t>
-  </si>
-  <si>
-    <t>eventID</t>
-  </si>
-  <si>
-    <t>institutionCode</t>
-  </si>
-  <si>
-    <t>institutionID</t>
-  </si>
-  <si>
-    <t>collectionCode</t>
-  </si>
-  <si>
-    <t>materialSampleID</t>
-  </si>
-  <si>
-    <t>associatedSequences</t>
-  </si>
-  <si>
-    <t>fieldNumber</t>
-  </si>
-  <si>
-    <t>catalogNumber</t>
-  </si>
-  <si>
-    <t>references</t>
-  </si>
-  <si>
-    <t>eventDate</t>
-  </si>
-  <si>
-    <t>samplingProtocol</t>
-  </si>
-  <si>
-    <t>locationID</t>
-  </si>
-  <si>
-    <t>decimalLatitude</t>
-  </si>
-  <si>
-    <t>decimalLongitude</t>
-  </si>
-  <si>
-    <t>geodeticDatum</t>
-  </si>
-  <si>
-    <t>coordinateUncertaintyInMeters</t>
-  </si>
-  <si>
-    <t>dataGeneralizations</t>
-  </si>
-  <si>
-    <t>recordedBy</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>municipality</t>
-  </si>
-  <si>
-    <t>verbatimLocality</t>
-  </si>
-  <si>
-    <t>minimumElevationInMeters</t>
-  </si>
-  <si>
-    <t>maximumElevationInMeters</t>
-  </si>
-  <si>
-    <t>minimumDepthInMeters</t>
-  </si>
-  <si>
-    <t>maximumDepthInMeters</t>
-  </si>
-  <si>
-    <t>16S_1</t>
-  </si>
-  <si>
-    <t>KTH</t>
-  </si>
-  <si>
-    <t>https://ror.org/026vcq606</t>
-  </si>
-  <si>
-    <t>https://www.ebi.ac.uk/ena/browser/view/SAMEA3724531</t>
-  </si>
-  <si>
-    <t>https://www.ebi.ac.uk/ena/browser/view/ERR1202034</t>
-  </si>
-  <si>
-    <t>some-catalogue-no</t>
-  </si>
-  <si>
-    <t>2013-07-13T07:08</t>
-  </si>
-  <si>
-    <t>200–500 mL seawater were filtered onto 0.22 μm pore-size mixed cellulose ester membrane filters; https://doi.org/10.3389/fmicb.2016.00679</t>
-  </si>
-  <si>
-    <t>EPSG:4326</t>
-  </si>
-  <si>
-    <t>Coordinates generalized from original GPS coordinates to three decimals</t>
-  </si>
-  <si>
-    <t>Arkona Basin</t>
-  </si>
-  <si>
-    <t>16S_2</t>
-  </si>
-  <si>
-    <t>https://www.ebi.ac.uk/ena/browser/view/SAMEA3724535</t>
-  </si>
-  <si>
-    <t>https://www.ebi.ac.uk/ena/browser/view/ERR1202038</t>
-  </si>
-  <si>
-    <t>2013-07-13T09:38</t>
-  </si>
-  <si>
-    <t>Baltic Proper</t>
-  </si>
-  <si>
-    <t>16S_3</t>
-  </si>
-  <si>
-    <t>https://www.ebi.ac.uk/ena/browser/view/SAMEA3724536</t>
-  </si>
-  <si>
-    <t>https://www.ebi.ac.uk/ena/browser/view/ERR1202039</t>
-  </si>
-  <si>
-    <t>2013-07-13T13:55</t>
-  </si>
-  <si>
-    <t>sop</t>
-  </si>
-  <si>
-    <t>target_gene</t>
-  </si>
-  <si>
-    <t>target_subfragment</t>
-  </si>
-  <si>
-    <t>lib_layout</t>
-  </si>
-  <si>
-    <t>seq_meth</t>
-  </si>
-  <si>
-    <t>pcr_primer_name_forward</t>
-  </si>
-  <si>
-    <t>pcr_primer_name_reverse</t>
-  </si>
-  <si>
-    <t>pcr_primer_forward</t>
-  </si>
-  <si>
-    <t>pcr_primer_reverse</t>
-  </si>
-  <si>
-    <t>denoising_appr</t>
-  </si>
-  <si>
-    <t>env_broad_scale</t>
-  </si>
-  <si>
-    <t>env_local_scale</t>
-  </si>
-  <si>
-    <t>env_medium</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.3389/fmicb.2016.00679</t>
-  </si>
-  <si>
-    <t>16S rRNA</t>
-  </si>
-  <si>
-    <t>V3-V4</t>
-  </si>
-  <si>
-    <t>paired</t>
-  </si>
-  <si>
-    <t>Illumina MiSeq</t>
-  </si>
-  <si>
-    <t>341F</t>
-  </si>
-  <si>
-    <t>805R</t>
-  </si>
-  <si>
-    <t>CCTACGGGNGGCWGCAG</t>
-  </si>
-  <si>
-    <t>GACTACHVGGGTATCTAATCC</t>
-  </si>
-  <si>
-    <t>DADA2</t>
-  </si>
-  <si>
-    <t>aquatic biome [ENVO_00002030]</t>
-  </si>
-  <si>
-    <t>marine biome [ENVO_00000447]</t>
-  </si>
-  <si>
-    <t>brackish water [ENVO_00002019]</t>
-  </si>
-  <si>
-    <t>measurementType</t>
-  </si>
-  <si>
-    <t>measurementTypeID</t>
-  </si>
-  <si>
-    <t>measurementValue</t>
-  </si>
-  <si>
-    <t>measurementValueID</t>
-  </si>
-  <si>
-    <t>measurementUnit</t>
-  </si>
-  <si>
-    <t>measurementUnitID</t>
-  </si>
-  <si>
-    <t>measurementAccuracy</t>
-  </si>
-  <si>
-    <t>measurementDeterminedDate</t>
-  </si>
-  <si>
-    <t>measurementDeterminedBy</t>
-  </si>
-  <si>
-    <t>measurementMethod</t>
-  </si>
-  <si>
-    <t>measurementRemarks</t>
-  </si>
-  <si>
-    <t>salinity</t>
-  </si>
-  <si>
-    <t>psu</t>
-  </si>
-  <si>
-    <t>temperature</t>
-  </si>
-  <si>
-    <t>°C</t>
-  </si>
-  <si>
-    <t>asv_id_alias</t>
-  </si>
-  <si>
-    <t>DNA_sequence</t>
-  </si>
-  <si>
-    <t>919a2aa9d306e4cf3fa9ca02a2aa5730</t>
-  </si>
-  <si>
-    <t>TCGAGAATTTTTCACAATGGGGGAAACCCTGATGGAGCGACGCCGCGTGGAGGATGAAGGTTTTCGGATTGTAAACTCCTGTCATTAGAGAACAAGGCACATGGTTTAACTGGCCGTGTGTTGATAGTATCTGAAGAGGAAGGGACGGCTAACTCTGTGCCAGCAGCCGCGGTAATACAGAGGTCTCAAGCGTTGTTCGGATTCATTGGGCGTAAAGGGTGCGTAGGTGGCGAGGTAAGTCGGATGTGAAATCTCCAAGCTCAACTTGGAAACTGCATTCGATACTGCTTTGCTAGAGGATTGTAGAGGGCATTGGAATTCACGGTGTAGCAGTGAAATGCGTAGATATCGTGAGGAAGACCAGTGGCGAAGGCGAATGCCTGGGCAATTCCTGACACTGAGGCACGAAGGCCAGGGGAGCAAACG</t>
-  </si>
-  <si>
-    <t>1ead98754d34073a4606f7ff1e94126e</t>
-  </si>
-  <si>
-    <t>TGGGGAATTTTCCGCAATGGGCGCAAGCCTGACGGAGCAACGCCGCGTGAGGGATGAAGGCCTCTGGGCTGTAAACCTCTTTTATCAAGGAAGAAGATCTGACGGTACTTGATGAATAAGCCACGGCTAATTCCGTGCCAGCAGCCGCGGTAATACGGGAGTGGCAAGCGTTATCCGGAATTATTGGGCGTAAAGCGTCCGCAGGCGGTTTTACAAGTCTGTCGTTAAAACGTGGAGCTCAACTCCATTTCGGCGATGGAAACTGTAAGACTAGAGTGTGGTAGGGGCAGAGGGAATTCCCGGTGTAGCGGTGAAATGCGTAGATATCGGGAAGAACACCAGTGGCGAAGGCGCTCTGCTGGGCCATAACTGACGCTCATGGACGAAAGCTAGGGGAGCGAAAG</t>
-  </si>
-  <si>
-    <t>43e088977eba5732bfa45e20b1d8cdd2</t>
-  </si>
-  <si>
-    <t>TCGAGAATTTTTCACAATGGGGGAAACCCTGATGGAGCGACGCCGCGTGGAGGATGAAGGTTTTCGGATCGTAAACTCCTGTCATTAGAGAACAAGGCACACGGTTTAACTGGCTGTGTGTTGATAGTATCTGAAGAGGAAGGGACGGCTAACTCTGTGCCAGCAGCCGCGGTAATACAGAGGTCTCAAGCGTTGTTCGGATTCATTGGGCGTAAAGGGTGCGTAGGTGGCGAGGTAAGTCGGATGTGAAATCTCCAAGCTCAACTTGGAAACTGCATTCGATACTGCTTTGCTAGAGGATTGTAGAGGGCATTGGAATTCACGGTGTAGCAGTGAAATGCGTAGATATCGTGAGGAAGACCAGTGGCGAAGGCGAATGCCTGGGCAATTCCTGACACTGAGGCACGAAGGCCAGGGGAGCAAACG</t>
-  </si>
-  <si>
-    <t>1b2c41577c16f4c672a2a861e6b89b14</t>
-  </si>
-  <si>
-    <t>TAGGGAATATTGGGCAATGGGCGAAAGCCTGACCCAGCGACGCCGCGTGAGGGATGAAGGTCTTCGGATTGTAAACCTCTTTCAGTAGGGAAGAAGCGAAAGTGACGGTACCTAAAGAAGAAGCACCGGCTAACTATGTGCCAGCAGCCGCGGTAATACATAGGGTGCAAGCGTTGTCCGGAATTATTGGGCGTAAAGAGCTCGTAGGTCGTTTGTCGCGTCGATTGTGAAAATCTGAGGCTCAACCTCAGACCTGCAGTCGATACGGGCAAACTAGAGTGTGGTAGGGGAGACTGGAATTCCTGGTGTAGCGGTGGAATGCGCAGATATCAGGAGGAACACCAATGGCGAAGGCAGGTCTCTGGGCCATAACTGACACTGAGGAGCGAAAGTGCGGGGAGCGAACA</t>
-  </si>
-  <si>
-    <t>40b37890b1b1fcdf0ece91f1da34c1ca</t>
-  </si>
-  <si>
-    <t>TGGGGAATTTTCCGCAATGGGCGCAAGCCTGACGGAGCAACGCCGCGTGAGGGATGAAGGCCTCTGGGCTGTAAACCTCTTTTATCAAGGAAGAAGATCTGACGGTACTTGATGAATAAGCCACGGCTAATTCCGTGCCAGCAGCCGCGGTAATACGGGAGTGGCAAGCGTTATCCGGAATTATTGGGCGTAAAGCGTCCGCAGGCGGTCTTGAAAGTCTGTTGTTAAAGCGTGGAGCTCAACTCCATTTCAGCAATGGAAACTAGAAGACTAGAGTGTGGTAGGGGCAGAGGGAATTCCCGGTGTAGCGGTGAAATGCGTAGATATCGGGAAGAACACCAGTGGCGAAGGCGCTCTGCTGGGCCATAACTGACGCTCATGGACGAAAGCCAGGGGAGCGAAAG</t>
-  </si>
-  <si>
-    <t>ae71bf7c99d3583a2d8841e5911c5716</t>
-  </si>
-  <si>
-    <t>TGGGGAATATTGGGCAATGGAGGAAACTCTGACCCAGCGACGCCGCGTGCGGGATGAAGGCCTTCGGGTTGTAAACCGCTTTCAGTAGGGAAGAAGCGAAAGTGACGGTACCTACAAAAGAAGCACCGGCTAACTATGTGCCAGCAGCCGCGGTAATACATAGGGTGCAAGCGTTGTCCGGAATTATTGGGCGTAAAGAGCTCGTAGGTCGTTTGTTACGTCGGATGTGAAAACCTGAGGCTCAACCTCAGGCCTGCATTCGATACGGGCAAACTAGAGTTTGGTAGGGGAGACTGGAATTCCTGGTGTAGCGGTGGAATGCGCAGATATCAGGAGGAACACCAATGGCGAAGGCAGGTCTCTGGGCCAATACTGACACTGAGGAGCGAAAGTCTGGGGAGCGAACA</t>
-  </si>
-  <si>
-    <t>887bc7033b46d960e893caceb711700b</t>
-  </si>
-  <si>
-    <t>TGGGGAATCTTGCGCAATGGGCGAAAGCCTGACGCAGCAACGCCGCGTGCGGGAAGAAGGCTTTCGGGCTGTAAACCGCTTTCAGCAGGAACGAAAATGACGGTACCTGCAGAAGAAGGAGCGGCCAACTATGTGCCAGCAGCCGCGGTGATACATAGGCTTCAAGCGTTGTCCGGATTTATTGGGCGTAAAGAGTTCGTAGGCGGTCGAGTAAGTCGGGTGTGAAAATTCTGGGCTCAACCCAGAGACGCCACCCGATACTGCTTAACTTGAGTTCGATAGGGGAGTGGGGAATTCCTAGTGTAGCGGTGAAATGCGCAGATATTAGGAGGAACACCGGTGGCGAAGGCGCCACTCTGGATCGACACTGACGCTGAGGAACGAAAGCATGGGTAGCAAACA</t>
-  </si>
-  <si>
-    <t>88b5b5240649749ca876d10823045b01</t>
-  </si>
-  <si>
-    <t>TGGGGAATCTTGCGCAATGGGCGAAAGCCTGACGCAGCAACGCCGCGTGCGGGATGAAGGCCTTCGGGCTGTAAACCGCTTTCAGCAGGAACGAAAATGACGGTACCTGCAGAAGAAGGAGCGGCCAACTACGTGCCAGCAGCCGCGGTGACACGTAGGCTCCAAGCGTTGTCCGGATTTATTGGGCGTAAAGAGCTCGTAGGCGGTTGAGTAAGTCGGGTGTGAAAACTCTGGGCTTAACCCGGAGACGCCATCCGATACTGCTCTGACTAGAGTTCAGGAGGGGAGTGGGGAATTCCTAGTGTAGCGGTGAAATGCGCAGATATTAGGAGGAACACCGGTGGCGAAGGCGCCACTCTGGACTGAAACTGACGCTGAGGAGCGAAAGCATGGGTAGCAAACA</t>
-  </si>
-  <si>
-    <t>95efad17b5fb6b91274a6ef3c47a098a</t>
-  </si>
-  <si>
-    <t>TGGGGAATTTTCCGCAATGGGCGCAAGCCTGACGGAGCAACGCCGCGTGAGGGATGAAGGCCTCTGGGCTGTAAACCTCTTTTATCAAGGAAGAAGATCTGACGGTACTTGATGAATAAGCCACGGCTAATTCCGTGCCAGCAGCCGCGGTAATACGGGAGTGGCAAGCGTTATCCGGAATTATTGGGCGTAAAGCGTCCGCAGGCGGTTTTACAAGTCTGTCGTTAAAACGTGGAGCTCAACTCCATTTCGGCGATGGAAACTGTAAGACTAGAGTGTGGTAGGGGCAGAGGGAATTCCCGGTGTAGCGGTGAAATGCGTAGATATCGGGAAGAACACCAGTGGCGAAGGCGCTCTGCTGGGCCATAACTGACGCTCATGGACGAAAGCCAGGGGAGCGAAAG</t>
-  </si>
-  <si>
-    <t>c366064866eaed18a54d15640272ab34</t>
-  </si>
-  <si>
-    <t>TGGGGAATATTGGGCAATGGAGGAAACTCTGACCCAGCGACGCCGCGTGCGGGATGAAGGCCTTCGGGTTGTAAACCGCTTTCAGCAGGGAAGAAGCGAAAGTGACGGTACCTGCAGAAGAAGCACCGGCTAACTATGTGCCAGCAGCCGCGGTAATACATAGGGTGCAAGCGTTGTCCGGAATTATTGGGCGTAAAGAGCTCGTAGGTGGTTCGTCACGTCGGATGTGAAACTCTGGGGCTTAACCCCAGACCTGCATTCGATACGGGCGAGCTTGAGTATGGTAGGGGAGTCTGGAATTCCTGGTGTAGCGGTGGAATGCGCAGATATCAGGAGGAACACCAATGGCGAAGGCAGGACTCTGGGCCATTACTGACACTGAGGAGCGAAAGCGTGGGGAGCGAACA</t>
-  </si>
-  <si>
-    <t>previous_identifications</t>
-  </si>
-  <si>
-    <t>organism_quantity</t>
-  </si>
-  <si>
-    <t>Bacteria|Verrucomicrobiota|Verrucomicrobiae|Chthoniobacterales|UBA6821|UBA6821|||</t>
-  </si>
-  <si>
-    <t>https://plutof.ut.ee/#/sequence/view/0000X0</t>
-  </si>
-  <si>
-    <t>Bacteria|Cyanobacteria|Cyanobacteriia|PCC-6307|Cyanobiaceae|Synechococcus_D|||</t>
-  </si>
-  <si>
-    <t>https://plutof.ut.ee/#/sequence/view/0000X1</t>
-  </si>
-  <si>
-    <t>Bacteria|Verrucomicrobiota|Verrucomicrobiae|Chthoniobacterales|||||</t>
-  </si>
-  <si>
-    <t>https://plutof.ut.ee/#/sequence/view/0000X2</t>
-  </si>
-  <si>
-    <t>Bacteria|Actinobacteriota|Actinomycetia|Nanopelagicales|Nanopelagicaceae|Nanopelagicus|||</t>
-  </si>
-  <si>
-    <t>https://plutof.ut.ee/#/sequence/view/0000X3</t>
-  </si>
-  <si>
-    <t>Bacteria|Cyanobacteria|Cyanobacteriia|PCC-6307|Cyanobiaceae|UBA5018|||</t>
-  </si>
-  <si>
-    <t>https://plutof.ut.ee/#/sequence/view/0000X4</t>
-  </si>
-  <si>
-    <t>https://plutof.ut.ee/#/sequence/view/0000X5</t>
-  </si>
-  <si>
-    <t>Bacteria|Actinobacteriota|Acidimicrobiia|Acidimicrobiales|Ilumatobacteraceae|BACL27|sp014190055||</t>
-  </si>
-  <si>
-    <t>https://plutof.ut.ee/#/sequence/view/0000X6</t>
-  </si>
-  <si>
-    <t>Bacteria|Actinobacteriota|Acidimicrobiia|Acidimicrobiales|Ilumatobacteraceae|UBA3006|||</t>
-  </si>
-  <si>
-    <t>https://plutof.ut.ee/#/sequence/view/0000X7</t>
-  </si>
-  <si>
-    <t>Bacteria|Cyanobacteria|Cyanobacteriia|PCC-6307|Cyanobiaceae||||</t>
-  </si>
-  <si>
-    <t>https://plutof.ut.ee/#/sequence/view/0000X8</t>
-  </si>
-  <si>
-    <t>Bacteria|Actinobacteriota|Actinomycetia|Nanopelagicales|Nanopelagicaceae|Planktophila|||</t>
-  </si>
-  <si>
-    <t>https://plutof.ut.ee/#/sequence/view/0000X9</t>
-  </si>
-  <si>
-    <t>asv_sequence</t>
-  </si>
-  <si>
-    <t>scientificName</t>
-  </si>
-  <si>
-    <t>taxonRank</t>
-  </si>
-  <si>
-    <t>kingdom</t>
-  </si>
-  <si>
-    <t>phylum</t>
-  </si>
-  <si>
-    <t>class</t>
-  </si>
-  <si>
-    <t>order</t>
-  </si>
-  <si>
-    <t>family</t>
-  </si>
-  <si>
-    <t>genus</t>
-  </si>
-  <si>
-    <t>specificEpithet</t>
-  </si>
-  <si>
-    <t>infraspecificEpithet</t>
-  </si>
-  <si>
-    <t>otu</t>
-  </si>
-  <si>
-    <t>annotation_confidence</t>
-  </si>
-  <si>
-    <t>date_identified</t>
-  </si>
-  <si>
-    <t>reference_db</t>
-  </si>
-  <si>
-    <t>annotation_algorithm</t>
-  </si>
-  <si>
-    <t>identification_references</t>
-  </si>
-  <si>
-    <t>taxon_remarks</t>
-  </si>
-  <si>
-    <t>annotation_target</t>
-  </si>
-  <si>
-    <t>target_criteria</t>
-  </si>
-  <si>
-    <t>target_prediction</t>
-  </si>
-  <si>
-    <t>JACTMZ01 sp018402585</t>
-  </si>
-  <si>
-    <t>species</t>
-  </si>
-  <si>
-    <t>Bacteria</t>
-  </si>
-  <si>
-    <t>Verrucomicrobiota</t>
-  </si>
-  <si>
-    <t>Verrucomicrobiae</t>
-  </si>
-  <si>
-    <t>Chthoniobacterales</t>
-  </si>
-  <si>
-    <t>JACTMZ01</t>
-  </si>
-  <si>
-    <t>sp018402585</t>
-  </si>
-  <si>
-    <t>SBDI-GTDB-R07-RS207-1 (https://scilifelab.figshare.com/articles/dataset/SBDI_Sativa_curated_16S_GTDB_database/14869077/4)</t>
-  </si>
-  <si>
-    <t>Ampliseq v2.5.0 (https://nf-co.re/ampliseq) DADA2:assignTaxonomy</t>
-  </si>
-  <si>
-    <t>https://docs.biodiversitydata.se/analyse-data/molecular-tools/#taxonomy-annotation</t>
-  </si>
-  <si>
-    <t>Domain = 'Bacteria'</t>
-  </si>
-  <si>
-    <t>Assigned kingdom OR barrnap-positive</t>
-  </si>
-  <si>
-    <t>Cyanobiaceae</t>
-  </si>
-  <si>
-    <t>Cyanobacteria</t>
-  </si>
-  <si>
-    <t>Cyanobacteriia</t>
-  </si>
-  <si>
-    <t>PCC-6307</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>MAG-120802 sp003569145</t>
-  </si>
-  <si>
-    <t>Actinobacteriota</t>
-  </si>
-  <si>
-    <t>Actinomycetia</t>
-  </si>
-  <si>
-    <t>Nanopelagicales</t>
-  </si>
-  <si>
-    <t>Nanopelagicaceae</t>
-  </si>
-  <si>
-    <t>MAG-120802</t>
-  </si>
-  <si>
-    <t>sp003569145</t>
-  </si>
-  <si>
-    <t>Ampliseq v2.5.0 (https://nf-co.re/ampliseq) DADA2:assignTaxonomy:addSpecies</t>
-  </si>
-  <si>
-    <t>Cyanobium_A sp015840335</t>
-  </si>
-  <si>
-    <t>Cyanobium_A</t>
-  </si>
-  <si>
-    <t>sp015840335</t>
-  </si>
-  <si>
-    <t>Nanopelagicus</t>
-  </si>
-  <si>
-    <t>BACL27 sp014190055</t>
-  </si>
-  <si>
-    <t>Acidimicrobiia</t>
-  </si>
-  <si>
-    <t>Acidimicrobiales</t>
-  </si>
-  <si>
-    <t>Ilumatobacteraceae</t>
-  </si>
-  <si>
-    <t>BACL27</t>
-  </si>
-  <si>
-    <t>sp014190055</t>
-  </si>
-  <si>
-    <t>UBA3006 sp002367695</t>
-  </si>
-  <si>
-    <t>UBA3006</t>
-  </si>
-  <si>
-    <t>sp002367695</t>
-  </si>
-  <si>
-    <t>Planktophila sp015660815</t>
-  </si>
-  <si>
-    <t>Planktophila</t>
-  </si>
-  <si>
-    <t>sp015660815</t>
-  </si>
-  <si>
-    <t>7ff490fff9504446139943d9c4f1be4a</t>
-  </si>
-  <si>
-    <t>TGGGGAATCTTGCGCAATGGGCGAAAGCCTGACGCAGCAACGCCGCGTGCGGGATGAAGGCCTTCGGGTTGTAAACCGCTTTCAGCAGGAACGAAAATGACGGTACCTGCAGAAGAAGGAGCGGCCAACTACGTGCCAGCAGCCGCGGTGACACGTAGGCTCCAAGCGTTGTCCGGATTTATTGGGCGTAAAGAGCTCGTAGGCGGTTTAGTAAGTCGGGTGTTAAAACTCTGGGCTCAACCCGGAGACGCCATCCGATACTACTATGACTTGAGTTCAGGAGGGGAGCGGGGAATTCCTAGTGTAGCGGTGAAATGCGCAGATATTAGGAGGAACACCGGTGGCGAAGGCGCCGCTCTGGACTGAAACTGACGCTGAGGAGCGAAAGCATGGGTAGCAAACA</t>
-  </si>
-  <si>
-    <t>96ff11f3fbe3bfe47f11753d3615eff9</t>
-  </si>
-  <si>
-    <t>TAAGGAATATTGGGCAATGGACGCAAGTCTGACCCAGCCATCCCGCGTGCAGGACGAATGCCCTATGGGTTGTAAACTGCTTTTGTTTGGGAAGAAATGTATTCTTTTAAGAGTATTTGACGGTACCAGACGAATAAGCACCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGTGCAAGCGTTATCCGGAATCACTGGGTTTAAAGGGTGCGTAGGCGGCCAGATAAGTCAGAGGTGAAAGTTTCCGGCTCAACCGGGAGATTGCCTTTGATACTGTTTGGCTTGAATCAGATTGAGGTTGGCGGAATGTGACATGTAGCGGTGAAATGCATAGATATGTCATAGAACATCGATTGCGAAGGCAGCTGGCTGGATCTGTATTGACGCTGAGGCACGAAAGCGTGGGGAGCAAACA</t>
-  </si>
-  <si>
-    <t>Saprospiraceae</t>
-  </si>
-  <si>
-    <t>Bacteroidota</t>
-  </si>
-  <si>
-    <t>Bacteroidia</t>
-  </si>
-  <si>
-    <t>Chitinophagales</t>
-  </si>
-  <si>
-    <t>60c5874530fb102c40f246e7b59cad1b</t>
-  </si>
-  <si>
-    <t>TAGGGAATCTTAGACAATGGGGGCAACCCTGATCTAGCCATGCCGCGTGTGTGATGAAGGCCCTAGGGTCGTAAAGCACTTTCGCCAGAGATGATAATGACAGTATCTGGTAAAGAAACCCCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGGGTTAGCGTTGTTCGGAATTACTGGGCGTAAAGCGCACGTAGGCGGATTAGTAAGTTAGAGGTGAAATCCCAGGGCTCAACCCTGGAACTGCCTTTAATACTGCTAGTCTTGAGTTCGAGAGAGGTAAGTGGAATTCCGAGTGTAGAGGTGAAATTCGTAGATATTCGGAGGAACACCAGTGGCGAAGGCGGCTTACTGGCTCGATACTGACGCTGAGGTGCGAAAGTGTGGGGAGCAAACA</t>
-  </si>
-  <si>
-    <t>Planktomarina</t>
-  </si>
-  <si>
-    <t>Proteobacteria</t>
-  </si>
-  <si>
-    <t>Alphaproteobacteria</t>
-  </si>
-  <si>
-    <t>Rhodobacterales</t>
-  </si>
-  <si>
-    <t>Rhodobacteraceae</t>
-  </si>
-  <si>
-    <t>cb8818c331eb97f13778cef034bb3af0</t>
-  </si>
-  <si>
-    <t>TGGGGAATCTTGCACAATGGGCGAAAGCCTGATGCAGCGATGCCGCGTGAGTGAAGAAGGCCTTTGGGTTGTAAAGCTCTTTTGTCGGGAAAGATAATGACTGTACCCGAAGAATAAGGTCCGGCTAACTTCGTGCCAGCAGCCGCGGTAATACGAAGGGACCTAGCGTAGTTCGGAATTACTGGGCGTAAAGAGTATGTAGGCGGCTAGATAAGTTAATTGTGAAAGCCCAAAGCTTAACTTTGGAATTGCAATTAAAACTATTTAGCTGGAGTATGATAGAGGAAAGCGGAATACATAGTGTAGAGGTGAAATTCGTAGATATTATGTAGAACACCAGTTGCGAAGGCGGCTTTCTGGATCATTACTGACGCTGAGATACGAAAGTATGGGTAGCGAAGA</t>
-  </si>
-  <si>
-    <t>IMCC9063 sp000750175</t>
-  </si>
-  <si>
-    <t>Pelagibacterales</t>
-  </si>
-  <si>
-    <t>Pelagibacteraceae</t>
-  </si>
-  <si>
-    <t>IMCC9063</t>
-  </si>
-  <si>
-    <t>sp000750175</t>
-  </si>
-  <si>
-    <t>53964bef6e413d0037100ef13b369504</t>
-  </si>
-  <si>
-    <t>TCGAGAATCTTCGGCAATGGGCGAAAGCCTGACCGAGCGATGCCGCGTGCGGGATGAAGGCCCTCGGGTTGTAAACCGCTGTCAACGAGGAGGAAGTGCAAGGGGGTTCTCCCTTTTGTTTGACCTATTCGAGAAGGAAGTACGGGCTAAGTTCGTGCCAGCAGCCGCGGTAAGACGAACCGTACAAACGTTATTCGGAATTATTGGGCTTAAAGGGTGCGTAGGCTGCGCGGAAAGTTGGGTGTGAAAGCCCTCGGCTCAACCGAGGAATTGCGCCCAAAACTACCGTGCTCGAGGGAGACAGAGGTGAGCGGAACTCAAGGTGGAGCGGTGAAATGCGTTGATATCTTGAGGAACACCGGTGGCGAAAGCGGCTCACTGGGTCTCTTCTGACGCTGAGGCACGAAAGCCAAGGTAGCAAACG</t>
-  </si>
-  <si>
-    <t>M30B53 sp018401745</t>
-  </si>
-  <si>
-    <t>Planctomycetota</t>
-  </si>
-  <si>
-    <t>Planctomycetia</t>
-  </si>
-  <si>
-    <t>Pirellulales</t>
-  </si>
-  <si>
-    <t>UBA1268</t>
-  </si>
-  <si>
-    <t>M30B53</t>
-  </si>
-  <si>
-    <t>sp018401745</t>
-  </si>
-  <si>
-    <t>766533668513f1de8efb46206dd0e235</t>
-  </si>
-  <si>
-    <t>TGGGGAATTTTCCGCAATGGGCGAAAGCCTGACGGAGCAACGCCGCGTGAGGGATGAAGGCCTCTGGGCTGTAAACCTCTTTTATCAAGGAAGAAGATCTGACGGTACTTGATGAATAAGCCACGGCTAATTCCGTGCCAGCAGCCGCGGTAATACGGGAGTGGCAAGCGTTATCCGGAATTATTGGGCGTAAAGCGTCCGCAGGCGGCCCAACAAGTCTGCTGTTAAAAAGTGGAGCTTAACTCCATCATGGCAGTGGAAACTGTTGGGCTAGAGTGTGGTAGGGGCAGAGGGAATTCCCGGTGTAGCGGTGAAATGCGTAGATATCGGGAAGAACACCAGTGGCGAAGGCGCTCTGCTGGGCCATCACTGACGCTCATGGACGAAAGCCAGGGGAGCGAAAG</t>
-  </si>
-  <si>
-    <t>Synechococcus_C sp014279835</t>
-  </si>
-  <si>
-    <t>Synechococcus_C</t>
-  </si>
-  <si>
-    <t>sp014279835</t>
-  </si>
-  <si>
-    <t>cac37e39df2461953f24398212940edf</t>
-  </si>
-  <si>
-    <t>TGAGGAATATTGGACAATGGGCGAGAGCCTGATCCAGCCATGCCGCGTGCAGGAAGACTGCCCTATGGGTTGTAAACTGCTTTTATACAGGAAGAATAAGCCTTACGTGTAAGGTGATGACGGTACTGTAAGAATAAGGACCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGTCCGAGCGTTATCCGGAATTATTGGGTTTAAAGGGTCCGTAGGCGGATGATTAAGTCAGGGGTGAAAGTTTGCAGCTCAACTGTAAAATTGCCTTTGATACTGGTCATCTTGAGTTGTATTGAAGTAGGCGGAATATGTAGTGTAGCGGTGAAATGCATAGATATTACATAGAACACCAATTGCGAAGGCAGCTTACTAAGTACTAACTGACGCTGATGGACGAAAGCGTGGGTAGCGAACA</t>
-  </si>
-  <si>
-    <t>MAG-120531 sp000173115</t>
-  </si>
-  <si>
-    <t>Flavobacteriales</t>
-  </si>
-  <si>
-    <t>Flavobacteriaceae</t>
-  </si>
-  <si>
-    <t>MAG-120531</t>
-  </si>
-  <si>
-    <t>sp000173115</t>
-  </si>
-  <si>
-    <t>73ec397d035244c7734fc7513050637d</t>
-  </si>
-  <si>
-    <t>TGGGGAATCTTGTGCAATGGACGAAAGTCTGACACAGCCACGCCGCGTGCGGGAAGAAGGCCTTCGGGTTGTAAACCGCTTTCAGCAGGAACGAAAATGACGGTACCTGCAGAAGAAGGAGCGGCCAACTACGTGCCAGCAGCCGCGGTGACACGTAGGCTCCAAGCGTTGTCCGGATTTATTGGGCGTAAAGAGCTCGTAGGCGGTTCAGCAAGTCGGGTGTGAAAACTCTGGGCTCAACCCAGAGCCTGCACCCGAAACTGCTGTGACTAGAGTTCGGTAGGGGAGTGGGGAATTCCTAGTGTAGCGGTGAAATGCGCAGATATTAGGAGGAACACCGATGGCGAAGGCACCACTCTGGGCCGAAACTGACGCTGAGGAGCGAAAGCGTGGGTAGCAAACA</t>
-  </si>
-  <si>
-    <t>UBA2093 sp903929185</t>
-  </si>
-  <si>
-    <t>UBA2093</t>
-  </si>
-  <si>
-    <t>sp903929185</t>
-  </si>
-  <si>
-    <t>d3a2fb3b65e96a6017a70182466040d8</t>
-  </si>
-  <si>
-    <t>TAGGGAATATTGGGCAATGGTCGCAAGACTGACCCAGCCATGCCGCGTGCAGGAAGACGGCCCTCTGGGTTGTAAACTGCTTTTATCTGGGAAGAAAAAGTCCATGCGTGGAAAATTGCCGGTACCAGATGAATAAGCACCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGTGCAAGCGTTGTCCGGATTTATTGGGTTTAAAGGGTGCGTAGGCGGCTGAATAAGTCAGCGGTGAAAGACTTCGGCTTAACCGGAGCAGTGCCGTTGATACTGTTTAGCTTGAGTGTTGGAGGGGTACATGGAATTGATGGTGTAGCGGTGAAATGCATAGATACCATCAGGAACACCGATAGCGAAGGCATTGTACTGGCCAACAACTGACGCTGAGGCACGAAAGTGTGGGGATCGAACA</t>
-  </si>
-  <si>
-    <t>Algoriphagus</t>
-  </si>
-  <si>
-    <t>Cytophagales</t>
-  </si>
-  <si>
-    <t>Cyclobacteriaceae</t>
-  </si>
-  <si>
-    <t>7208feb3afd481ebd51c04bb97e20644</t>
-  </si>
-  <si>
-    <t>TGGGGAATCTTAGACAATGGGCGCAAGCCTGATCTAGCCATGCCGCGTGAGCGATGAAGGCCTTAGGGTTGTAAAGCTCTTTCAGTGGGGAAGATAATGACGGTACCCACAGAAGAAGCCCCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGGGCTAGCGTTGTTCGGAATTACTGGGCGTAAAGCGCGCGTAGGCGGATTGGAAAGTTGGAGGTGAAATCCCAGGGCTCAACCTTGGAACTGCCTTCAAAACTTCCAGTCTGGAGTTCGAGAGAGGTGAGTGGAATTCCGAGTGTAGAGGTGAAATTCGTAGATATTCGGAGGAACACCAGTGGCGAAGGCGGCTCACTGGCTCGATACTGACGCTGAGGTGCGAAAGCGTGGGGAGCAAACA</t>
-  </si>
-  <si>
-    <t>3451a03945f809e8f5d5a86e2d914717</t>
-  </si>
-  <si>
-    <t>TGAGGAATATTGGGCAATGGAGGCAACTCTGACCCAGCTATGCCGCGTGCAGGAAGACGGCCCTCTGGGTTGTAAACTGCTTTTGTTTGGGAATAAACCCTCCTACGTGTAGGAGGCTGAAGGTACCTTACGAATAAGCATCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGATGCAAGCGTTATCCGGATTTATTGGGTTTAAAGGGTCCGTAGGCGGATCTTTAAGTCAGTGGTGAAAGCCCACAGCTCAACTGTGGAACTGCCATTGATACTGGAGATCTTGAGTGTAGTAGAAGTAGGCGGAATAGGGCATGTAGCGGTGAAATGCATAGATATGCCCTAGAACACCGATTGCGAAGGCAGCTTACTATGTTACAACTGACGCTGAGGGACGAAAGCGTGGGGAGCAAACA</t>
-  </si>
-  <si>
-    <t>TMED14 sp016868755</t>
-  </si>
-  <si>
-    <t>Schleiferiaceae</t>
-  </si>
-  <si>
-    <t>TMED14</t>
-  </si>
-  <si>
-    <t>sp016868755</t>
-  </si>
-  <si>
-    <t>f7600dd883bbcd817ee6cc47d0f7ee56</t>
-  </si>
-  <si>
-    <t>TGAGGAATATTGGACAATGGGCGCAAGCCTGATCCAGCCATGCCGCGTGCAGGAAGACGGTCCTATGGATTGTAAACTGCTTTTATACAGGAAGAAACAACTCTACGTGTAGAGTCTTGACGGTACTGTAGGAATAAGGATCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGATCCAAGCGTTATCCGGAATCATTGGGTTTAAAGGGTCCGTAGGCGGTCTTATAAGTCAGTGGTGAAATCTCCTAGCTCAACTAGGAAACTGCCATTGATACTGTAAGACTTGAATTTTTGTGAAGTAACTAGAATATGTAGTGTAGCGGTGAAATGCTTAGATATTACATGGAATACCAATTGCGAAGGCAGGTTACTAACAAACGATTGACGCTGATGGACGAAAGCGTGGGGAGCGAACA</t>
-  </si>
-  <si>
-    <t>Flavobacterium</t>
-  </si>
-  <si>
-    <t>eddec92462c6800adb4026d680198cb7</t>
-  </si>
-  <si>
-    <t>TGGGGAATTTTCCGCAATGGGCGAAAGCCTGACGGAGCAACGCCGCGTGAGGGATGAAGGCCTCTGGGCTGTAAACCTCTTTTATCAAGGAAGAAGATCTGACGGTACTTGATGAATAAGCCACGGCTAATTCCGTGCCAGCAGCCGCGGTAATACGGGAGTGGCAAGCGTTATCCGGAATTATTGGGCGTAAAGCGTCCGCAGGCGGCCCTTCAAGTCTGCTGTTAAAAAGTGGAGCTTAACTCCATCATGGCAGTGGAAACTGAGGGGCTTGAGTGTGGTAGGGGCAGAGGGAATTCCCGGTGTAGCGGTGAAATGCGTAGATATCGGGAAGAACACCAGTGGCGAAGGCGCTCTGCTGGGCCATCACTGACGCTCATGGACGAAAGCCAGGGGAGCGAAAG</t>
-  </si>
-  <si>
-    <t>Synechococcus_E</t>
-  </si>
-  <si>
-    <t>55060bfb51dc35530beac964e48e44bd</t>
-  </si>
-  <si>
-    <t>TCGAGGATTTTTCTCAATGGGGGCAACCCTGAAGGAGCGACGCCGCGTGGAGGATGAAGGGCTTCGGCTCGTAAACTCCTGTCACCGACGAACAAGGCATCCGGATTAATAAATCGGATGCTTGATGGTAGTCGGAGAGGAAGGGGCGGCTAACTCTGTGCCAGCAGCCGCGGTGATACAGAGGCCCCAAGCGTTGTTCGGATTTACTGGGCGTAAAGGGTGTGTAGGGGGTCGGGTAAGTTTGACGTGAAATCCCGTTGCTCAACAACGGAACTGCGTCGAATACTGCTCGGCTGGAGGTTCGGAGATGAGGGCGGAATTCTCGGTGTAGCGGTGAAATGCGTAGATATCGAGAGGAACGCCGACGGCGAAAGCAGCCCTCAAGACGAAATCTGACCCTGAAACACGAAGGCCAGGGGAGCAAACG</t>
-  </si>
-  <si>
-    <t>UBA3015 sp001438005</t>
-  </si>
-  <si>
-    <t>Methylacidiphilales</t>
-  </si>
-  <si>
-    <t>UBA3015</t>
-  </si>
-  <si>
-    <t>sp001438005</t>
-  </si>
-  <si>
-    <t>9ac1d376f84dff0b4a0b11b609620bfa</t>
-  </si>
-  <si>
-    <t>TGGGGAATCTTAGACAATGGGCGCAAGCCTGATCTAGCCATGCCGCGTGAGTGATGAAGGCCTTAGGGTCGTAAAGCTCTTTCGCCTGTGATGATAATGACAGTAGCAGGTAAAGAAACCCCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGGGTTAGCGTTGTTCGGAATTACTGGGCGTAAAGCGCACGTAGGCGGATTGGAAAGTTGGGGGTGAAATCCCGGGGCTCAACCCCGGAACTGCCTCCAAAACTATCAGTCTAGAGTTCGAGAGAGGTGAGTGGAATTCCAAGTGTAGAGGTGAAATTCGTAGATATTTGGAGGAACACCAGTGGCGAAGGCGGCTCACTGGCTCGATACTGACGCTGAGGTGCGAAAGTGTGGGGAGCAAACA</t>
-  </si>
-  <si>
-    <t>LGRT01</t>
-  </si>
-  <si>
-    <t>aaf363d33b413559f355276afbb79f37</t>
-  </si>
-  <si>
-    <t>TGGGGAATCTTAGACAATGGGCGCAAGCCTGATCTAGCCATGCCGCGTGATCGATGAAGGCCTTAGGGTTGTAAAGATCTTTCAGTTGGGAAGATAATGACGGTACCAACAGAAGAAGCCCCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGGGCTAGCGTTATTCGGAATTACTGGGCGTAAAGCGCACGTAGGCGGATTAGAAAGTCAGAGGTGAAATCCCAGGGCTCAACCTTGGAACTGCCTTTGAAACTTCTAGTCTTGAGTTCGAGAGAGGTGAGTGGAATTCCGAGTGTAGAGGTGAAATTCGTAGATATTCGGAGGAACACCAGTGGCGAAGGCGGCTCACTGGCTCGATACTGACGCTGAGGTGCGAAAGCGTGGGGAGCAAACA</t>
-  </si>
-  <si>
-    <t>UBA10365 sp003536295</t>
-  </si>
-  <si>
-    <t>UBA10365</t>
-  </si>
-  <si>
-    <t>sp003536295</t>
-  </si>
-  <si>
-    <t>19b76dc633050df9ec212f0995316cbd</t>
-  </si>
-  <si>
-    <t>TGGGGAATTTTGGACAATGGGCGAAAGCCTGATCCAGCAATGCCGCGTGTGCGAAGAAGGCCTTCGGGTTGTAAAGCACTTTTGTCAGGAAAGAAATTGTTCGGGCCAATACCCCGAGCCGTTGACGGTACCTGAAGAATAAGCACCGGCTAACTACGTGCCAGCAGCCGCGGTAATACGTAGGGTGCGAGCGTTAATCGGAATTACTGGGCGTAAAGCGTGCGCAGGCGGTTTGTTAAGACAGTTGTGAAATCCCCGGGCTCAACCTGGGAACTGCAATTGTGACTGGCAGGCTAGAGTTTGGCAGAGGGGGGTGGAATTCCTGGTGTAGCAGTGAAATGCGTAGATATCAGGAGGAACACCGATGGCGAAGGCAGCCCCCTGGGCCATGACTGACGCTCATGCACGAAAGCGTGGGGAGCAAACA</t>
-  </si>
-  <si>
-    <t>UBA2463 sp018402635</t>
-  </si>
-  <si>
-    <t>Gammaproteobacteria</t>
-  </si>
-  <si>
-    <t>Burkholderiales</t>
-  </si>
-  <si>
-    <t>Burkholderiaceae</t>
-  </si>
-  <si>
-    <t>UBA2463</t>
-  </si>
-  <si>
-    <t>sp018402635</t>
-  </si>
-  <si>
-    <t>3170f6094605a579e6a0e1fefd33a2a5</t>
-  </si>
-  <si>
-    <t>TGGGGAATCTTAGACAATGGGCGCAAGCCTGATCTAGCCATGCCGCGTGAGTGACGAAGGCCTTAGGGTCGTAAAGCTCTTTCGCCAGAGATGATAATGACAGTATCTGGTAAAGAAACCCCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGGGTTAGCGTTGTTCGGAATTACTGGGCGTAAAGCGCACGTAGGCGGATTGGAAAGTATGGGGTGAAATCCCAGGGCTCAACCCTGGAACGGCCTTGTAAACTCCCAGTCTAGAGTTCGAGAGAGGTGAGTGGAATTCCAAGTGTAGAGGTGAAATTCGTAGATATTTGGAGGAACACCAGTGGCGAAGGCGGCTCACTGGCTCGATACTGACGCTGAGGTGCGAAAGTGTGGGGAGCAAACA</t>
-  </si>
-  <si>
-    <t>Yoonia</t>
-  </si>
-  <si>
-    <t>21bf8c2fc46ed6c2534c698b98cc683b</t>
-  </si>
-  <si>
-    <t>TGGGGAATTTTGGACAATGGGCGCAAGCCTGATCCAGCCATGCCGCGTGCAGGATGAAGGCCTTCGGGTTGTAAACTGCTTTTGTACGGAACGAAAAGGTTTGGCCTAATAAGCTGGACCCATGACGGTACCGTAAGAATAAGCACCGGCTAACTACGTGCCAGCAGCCGCGGTAATACGTAGGGTGCGAGCGTTAATCGGAATTACTGGGCGTAAAGCGTGCGCAGGCGGTTATGTAAGACAGATGTGAAATCCCCGGGCTCAACCTGGGAACTGCATTAGTGACTGCATAGCTGGAGTACGGCAGAGGGGGATGGAATTCCGCGTGTAGCAGTGAAATGCGTAGATATGCGGAGGAACACCGATGGCGAAGGCAATCCCCTGGGCCTGTACTGACGCTCATGCACGAAAGCGTGGGGAGCAAACA</t>
-  </si>
-  <si>
-    <t>Curvibacter gracilis</t>
-  </si>
-  <si>
-    <t>Curvibacter</t>
-  </si>
-  <si>
-    <t>gracilis</t>
-  </si>
-  <si>
-    <t>cc87cf7731ae4eb54c4d6a8169d4598e</t>
-  </si>
-  <si>
-    <t>TGGGGAATCTTGCGCAATGGGCGAAAGCCTGACGCAGCAACGCCGCGTGCGGGATGAAGGCCTTCGGGCTGTAAACCGCTTTCAGCAGGAACGAAAATGACGGTACCTGCAGAAGAAGGAGCGGCCAACTACGTGCCAGCAGCCGCGGTGACACGTAGGCTCCAAGCGTTGTCCGGATTTATTGGGCGTAAAGAGCTCGTAGGCGGTTTAGTAAGTCGGGTGTGAAAACTCTGGGCTTAACCCGGAGACGCCATCCGATACTGCTATGACTTGAGTTCAGGAGGGGAGCGGGGAATTCCTAGTGTAGCGGTGAAATGCGCAGATATTAGGAGGAACACCGGTGGCGAAGGCGCCGCTCTGGACTGAAACTGACGCTGAGGAGCGAAAGCATGGGTAGCAAACA</t>
-  </si>
-  <si>
-    <t>0aa4663de19d33cbaec31569d47cf191</t>
-  </si>
-  <si>
-    <t>TGAGGAATATTGGTCAATGGGCGCAAGCCTGAACCAGCCATGCCGCGTGCAGGAAGAATGCCCTATGGGTTGTAAACTGCTTTTATTTGGGAATAAACCTCTTTACGTGTAGAGAGCTGAAGGTACCAAATGAATAAGCACCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGTGCAAGCGTTATCCGGAATCATTGGGTTTAAAGGGTCCGCAGGCGGATTTATAAGTCAGTGGTGAAATCCTATCGCTTAACGATAGAACTGCCATTGATACTGTAAGTCTTGAATTCGGTCGGAGTGGGCGGAATGTGTAGTGTAGCGGTGAAATGCATAGATATTACACAGAACACCGATAGCGAAGGCAGCTCACTAGGCCTGAATTGACGCTCAGGGACGAAAGCGTGGGGATCAAACA</t>
-  </si>
-  <si>
-    <t>UBA952 sp016872115</t>
-  </si>
-  <si>
-    <t>Crocinitomicaceae</t>
-  </si>
-  <si>
-    <t>UBA952</t>
-  </si>
-  <si>
-    <t>sp016872115</t>
-  </si>
-  <si>
-    <t>ac4107604c179f2f8414333885255725</t>
-  </si>
-  <si>
-    <t>TGGGGAATTTTCCGCAATGGGCGAAAGCCTGACGGAGCAATACCGCGTGAGGGAGGAAGGCTCTTGGGTTGTAAACCTCTTTTCTCAGGGAAGAACAGAATGACGGTACCTGAGGAATAAGCATCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGATGCAAGCGTTATCCGGAATGATTGGGCGTAAAGGGTCCGCAGGTGGCATTGTAAGTCTGCTGTTAAAGAGTTTGGCTCAACCAAATAAGAGCAGTGGAAACTACAAAGCTAGAGTGTGGTCGGGGCAGAGGGAATTCCTGGTGTAGCGGTGAAATGCGTAGATATCAGGAAGAACACCAGTGGCGAAGGCGCTCTGCTAGGCCGAGACTGACACTGAGGGACGAAAGCTAGGGGAGCGAATG</t>
-  </si>
-  <si>
-    <t>Dolichospermum flosaquae</t>
-  </si>
-  <si>
-    <t>Cyanobacteriales</t>
-  </si>
-  <si>
-    <t>Nostocaceae</t>
-  </si>
-  <si>
-    <t>Dolichospermum</t>
-  </si>
-  <si>
-    <t>flosaquae</t>
-  </si>
-  <si>
-    <t>380d81417892576cb8aa4c50e92e5e1d</t>
-  </si>
-  <si>
-    <t>TGAGGAATATTGGGCAATGGAGGCAACTCTGACCCAGCCATGCCGCGTGCAGGAATAAGGTCCTATGGATTGTAAACTGCTTTTATACAGGAAGAAACACTCGGACGTGTCCGAGCTTGACGGTACTGTATGAATAAGCACCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGTGCAAGCGTTATCCGGAATCATTGGGTTTAAAGGGTCCGCAGGCGGTCAATTAAGTCAGAGGTGAAATCCCATCGCTTAACGATGGAACTGCCTTTGATACTGGTTGACTTGAGTCATATGGAAGTAGATAGAATGTGTAGTGTAGCGGTGAAATGCATAGATATTACACAGAATACCGATTGCGAAGGCAGTCTACTACGTATGTACTGACGCTCATGGACGAAAGCGTGGGGAGCGAACA</t>
-  </si>
-  <si>
-    <t>Polaribacter</t>
-  </si>
-  <si>
-    <t>b15dce65a0a29efb0bcfadedd72ede3c</t>
-  </si>
-  <si>
-    <t>TGGGGAATATTGGGCAATGGAGGGAACTCTGACCCAGCGACGCCGCGTGCGGGATGAAGGCCTTCGGGTTGTAAACCGCTTTCAGCAAGGAAGAAGCGAAAGTGACGGTACTTGCAGAAGAAGCACCGGCTAACTATGTGCCAGCAGCCGCGGTAATACATAGGGTGCAAGCGTTGTCCGGAATTATTGGGCGTAAAGAGCTCGTAGGTGGTTCGTCACGTCGGATGTGAAAATCTGGGGCTTAACCCCAGACCTGCATTCGATACGGGCGAGCTAGAGTGTGGTAGGGGAGACTGGAATTCCTGGTGTAGCGGTGGAATGCGCAGATATCAGGAGGAACACCAATGGCGAAGGCAGGTCTCTGGGCCATTACTGACACTGAGGAGCGAAAGCGTGGGGAGCGAACA</t>
-  </si>
-  <si>
-    <t>5d12a2cd51bf17060f60270529c5722e</t>
-  </si>
-  <si>
-    <t>TGGGGAATATTGGACAATGGGCGCAAGCCTGATCCAGCCATGCCGCGTGTGTGAAGAAGGCTCTAGGGTTGTAAAGCACTTTCAGTAGGGAGGAAGGCCAGAGTGTTAATAGCGCTTTGGATTGACGTTACCTACAGAAGCAGCACCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGTGCAAGCGTTAATCGGAATTACTGGGCGTAAAGCGCGCGTAGGCGGTTTGTTAAGTGTGATGTGAAAGCCCAGGGCTCAACCTTGGAACTGCATCACATACTGGCAAGCTAGAGTACGGTAGAGGGGGGTAGAATTCCATGTGTAGCGGTGAAATGCGTAGAGATGTGGAGGAATACCAGTGGCGAAGGCGGCCCCCTGGATCGATACTGACGCTGAGGTGCGAAAGCGTGGGGAGCAAACA</t>
-  </si>
-  <si>
-    <t>UBA9145 sp001438145</t>
-  </si>
-  <si>
-    <t>Pseudomonadales</t>
-  </si>
-  <si>
-    <t>Pseudohongiellaceae</t>
-  </si>
-  <si>
-    <t>UBA9145</t>
-  </si>
-  <si>
-    <t>sp001438145</t>
-  </si>
-  <si>
-    <t>ff9f5d078bc5ba693575630c8cdaef70</t>
-  </si>
-  <si>
-    <t>TGGGGAATTTTGGACAATGGGCGCAAGCCTGATCCAGCAATGCCGCGTGAGTGAAGAAGGCCTTCGGGTTGTAAAGCTCTTTTGTCAGGGAAGAAACGGTGAGAGCTAATATCTTTTGCTAATGACGGTACCTGAAGAATAAGCACCGGCTAACTACGTGCCAGCAGCCGCGGTAATACGTAGGGTGCAAGCGTTAATCGGAATTACTGGGCGTAAAGCGTGCGCAGGCGGTTATGTAAGACAGATGTGAAATGCCCGGGCTTAACCTGGGAACTGCATTTGTGACTGCATGGCTAGAGTGTGTCAGAGGGGGGTAGAATTCCACGTGTAGCAGTGAAATGCGTAGATATGTGGAGGAATACCGATGGCGAAGGCAGCCCCCTGGGATAACACTGACGCTCATGCACGAAAGCGTGGGGAGCAAACA</t>
-  </si>
-  <si>
-    <t>Herbaspirillum sp004134995</t>
-  </si>
-  <si>
-    <t>Herbaspirillum</t>
-  </si>
-  <si>
-    <t>sp004134995</t>
-  </si>
-  <si>
-    <t>272f79649c2702bec9ff272552ffffcf</t>
-  </si>
-  <si>
-    <t>TGGGGAATTTTCCGCAATGGGCGAAAGCCTGACGGAGCAACGCCGCGTGAGGGATGAAGGCCTCTGGGCTGTAAACCTCTTTTATCAAGGAAGAAGATCTGACGGTACTTGATGAATAAGCCACGGCTAATTCCGTGCCAGCAGCCGCGGTAATACGGGAGTGGCAAGCGTTATCCGGAATTATTGGGCGTAAAGCGTCCGCAGGCGGTCTTGTAAGTCTGTCGTTAAAGCGTGGAGCTTAACTCCATTTCGGCGGTGGAAACTACAAGACTAGAGTGTGGTAGGGGCAGAGGGAATTCCCGGTGTAGCGGTGAAATGCGTAGATATCGGGAAGAACACCAGTGGCGAAGGCGCTCTGCTGGGCCATAACTGACGCTCATGGACGAAAGCCAGGGGAGCGAAAG</t>
-  </si>
-  <si>
-    <t>7c11f640776d5482ec95173ca61de908</t>
-  </si>
-  <si>
-    <t>TGGGGAATATTGCGCAATGGGCGAAAGCCTGACGCAGCAACGCCGCGTGAGGGATGACGGCCTTCGGGTTGTAAACCTCTTTCAGCAGGGAAGAAGCGAGAGTGACGGTACCTGCAGAAGAAGCACCGGCTAACTACGTGCCAGCAGCCGCGGTAATACGTAGGGTGCAAGCGTTGTCCGGATTTATTGGGCGTAAAGAGCTCGTAGGCGGTTAGTCGCGTCGGATGTGAAATCCTAGAGCTTAACTCTGGGCCTGCATTCGATACGGGCTGACTCGAGTATTGTAGGGGAGACTGGAACTCCTGGTGTAGCGGTGAAATGCGCAGATATCAGGAAGAACACCGGTGGCGAAGGCGGGTCTCTGGGCAATTACTGACGCTGAGGAGCGAAAGCGTGGGGAGCAAACA</t>
-  </si>
-  <si>
-    <t>S36-B12</t>
-  </si>
-  <si>
-    <t>bfbb41fc686730dd0f3e13df27759598</t>
-  </si>
-  <si>
-    <t>TGGGGAATCTTAGACAATGGGGGAAACCCTGATCTAGCCATGCCGCGTGAGTGACGAAGGCCTTAGGGTCGTAAAGCTCTTTCACCAGGGATGATAATGACAGTACCTGGAGAAGAAACCCCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGGGTTAGCGTTGTTCGGAATTACTGGGCGTAAAGCGCACGTAGGCGGATTAGTCAGTCAGAGGTGAAATCCCAGGGCTCAACCTTGGAACTGCCTTTGATACTGCTAGTCTTGAGTTCGAGAGAGGTGAGTGGAATTCCGAGTGTAGAGGTGAAATTCGTAGATATTCGGAGGAACACCAGTGGCGAAGGCGGCTCACTGGCTCGATACTGACGCTGAGGTGCGAAAGCGTGGGGAGCAAACA</t>
-  </si>
-  <si>
-    <t>Roseicyclus sp015689735</t>
-  </si>
-  <si>
-    <t>Roseicyclus</t>
-  </si>
-  <si>
-    <t>sp015689735</t>
-  </si>
-  <si>
-    <t>1505e5de35661b77871b454a575c128a</t>
-  </si>
-  <si>
-    <t>TCGAGAATAATTCACAATGGGGGCAACCCTGATGGTGCAACGCCGCGTGGAGGATGACGGTCTTCGGATTGTAAACTCCTGTCATCTGGGAGAAAGACCTGGCCGTTAATAGCGGACAGGGTTGATAGTACCAGAAGAGGAAGGGACGGCTAACTTCGTGCCAGCAGCCGCGGTAATACGAAGGTCCCAAGCGTTGTTCGGAATCACTGGGCGTAAAGGGAGCGTAGGCGGCGCGGTAAGTCAGATGTGAAATCCCGGGGCTCAACCCCGGAACTGCATCCGATACTGCCGTGCTTGAGCAATGGAGAGGTAGCTGGAATTATCGGTGTAGCAGTGAAATGCGTAGATATCGATAGGAACACTCGTGGCGAAAGCGAGCTACTGGACATTTGCTGACGCTGAGGCTCGAAGGCTAGGGGAGCGAAAG</t>
-  </si>
-  <si>
-    <t>Luteolibacter sp018402445</t>
-  </si>
-  <si>
-    <t>Verrucomicrobiales</t>
-  </si>
-  <si>
-    <t>Akkermansiaceae</t>
-  </si>
-  <si>
-    <t>Luteolibacter</t>
-  </si>
-  <si>
-    <t>sp018402445</t>
-  </si>
-  <si>
-    <t>1424204d0b3becbb64ef0b61abb46473</t>
-  </si>
-  <si>
-    <t>TGGGGAATTTTCCGCAATGGGCGCAAGCCTGACGGAGCAACGCCGCGTGAGGGACGAAGGCCTCTGGGCTGTAAACCTCTTTTCTCAAGGAAGAAGACATGACGGTACTTGAGGAATAAGCCACGGCTAATTCCGTGCCAGCAGCCGCGGTAATACGGGAGTGGCAAGCGTTATCCGGAATTATTGGGCGTAAAGCGTCCGCAGGCGGCCCAGCAAGTCTGTTGTTAAAAAGTGGAGCTCAACTCCATCCAGGCAATGGAAACTGCTGGGCTAGAGTGTGGTAGGGGCAGAGGGAATTCCCGGTGTAGCGGTGAAATGCGTAGATATCGGGAAGAACACCAGTGGCGAAGGCGCTCTGCTGGGCCATAACTGACGCTCATGGACGAAAGCCAGGGGAGCGAAAG</t>
-  </si>
-  <si>
-    <t>MW101C3 sp002252635</t>
-  </si>
-  <si>
-    <t>MW101C3</t>
-  </si>
-  <si>
-    <t>sp002252635</t>
-  </si>
-  <si>
-    <t>a7e194b4ea4b1df360fce3d3770d58ee</t>
-  </si>
-  <si>
-    <t>TGGGGAATCTTGCGCAATGGGCGAAAGCCTGACGCAGCAACGCCGCGTGCGGGAAGAAGGCCTTAGGGTTGTAAACCGCTTTCAGCAGGGAAGAAAATGACTGTACCTGCAGAAGAAGGTGCGGCCAACTACGTGCCAGCAGCCGCGGTGACACGTAGGCACCAAGCGTTGTCCGGATTTATTGGGCGTAAAGAGCTCGTAGGCTGTTCAGTTAGTTGGGTGTGAAAACTCCGGGCTTAACCCGGAGCCGCCACCCAATACTGCTGTGACTAGAGTTCGGTAGGGGAGCGGGGAATTCCTAGTGTAGCGGTGAAATGCGCAGATATTAGGAGGAACACCGGTGGCGAAGGCGCCGCTCTGGGCCGAAACTGACGCTGAGGAGCGAAAGCATGGGTAGCAAACA</t>
-  </si>
-  <si>
-    <t>c750452151a7570b94c64f9fcb207d33</t>
-  </si>
-  <si>
-    <t>TGAGGAATATTGGTCAATGGGCGCAAGCCTGAACCAGCCATGCCGCGTGCAGGAAGAATGCCCTATGGGTTGTAAACTGCTTTTATTTAGGAATAAACCTTTCTACGTGTAGAAAGCTGAAGGTACTGAATGAATAAGCACCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGTGCAAGCGTTATCCGGAATCATTGGGTTTAAAGGGTCCGCAGGCGGGCGTATAAGTCAGTGGTGAAATCCTGCAGCTTAACTGCAGAACTGCCATTGATACTGTACGTCTTGAATTCGGTCGAAGTGGGCGGAATGTGTAGTGTAGCGGTGAAATGCATAGATATTACACAGAACACCGATAGCGAAGGCAGCTCACTAGGCCTGGATTGACGCTCAGGGACGAAAGCGTGGGGATCAAACA</t>
-  </si>
-  <si>
-    <t>UBA952 sp009926125</t>
-  </si>
-  <si>
-    <t>sp009926125</t>
-  </si>
-  <si>
-    <t>93185103563e99d5dbd1111548078ed7</t>
-  </si>
-  <si>
-    <t>TGGGGAATTTTGGACAATGGGCGAAAGCCTGATCCAGCCATTCCGCGTGCAGGATGAAGGCCCTCGGGTTGTAAACTGCTTTTGTACAGAACGAAAAGGTTTCTATTAATACTAGGAGCTCATGACGGTACTGTAAGAATAAGCACCGGCTAACTACGTGCCAGCAGCCGCGGTAATACGTAGGGTGCAAGCGTTAATCGGAATTACTGGGCGTAAAGCGTGCGCAGGCGGTTATATAAGTCAGATGTGAAATCCCCGGGCTCAACCTGGGAACTGCATTTGAGACTGTATAGCTAGAGTACGGTAGAGGGGGATGGAATTCCGCGTGTAGCAGTGAAATGCGTAGATATGCGGAGGAACACCGATGGCGAAGGCAATCCCCTGGACCTGTACTGACGCTCATGCACGAAAGCGTGGGGAGCAAACA</t>
-  </si>
-  <si>
-    <t>56fa1dafeb007219a436225686b03582</t>
-  </si>
-  <si>
-    <t>TCGAGGATTTTTCTCAATGGGGGCAACCCTGAAGGAGCGACGCCGCGTGGAGGATGAAGGGCTTCGGCTCGTAAACTCCTGTCACCGACGAACAAGGCATTCGGATTAATAAATCGGATGCTTGATGGTAGTCGGAGAGGAAGGGGCGGCTAACTCTGTGCCAGCAGCCGCGGTGATACAGAGGCCCCAAGCGTTGTTCGGATTTACTGGGCGTAAAGGGTGTGTAGGGGGTTGGGTAAGTTTGACGTGAAATCCCGTTGCTCAACAACGGAACTGCGTCGAATACTGCTCAGCTGGAGGTTCGGAGATGAGGGCGGAATTCTCGGTGTAGCGGTGAAATGCGTAGATATCGAGAGGAACGCCGATGGCGAAAGCAGCCCTCAAGACGAAATCTGACCCTGAAACACGAAGGCCAGGGGAGCAAACG</t>
-  </si>
-  <si>
-    <t>458a614d9f091f772f92f51236d1105a</t>
-  </si>
-  <si>
-    <t>TGAGGAATATTGGTCAATGGGCGCAAGCCTGAACCAGCCATGCCGCGTGCAGGAAGACGGTCCTATGGATTGTAAACTGCTTTTATACAGGAAGAAACCCTCCCACGTGTGGGAGATTGACGGTACTGTAGGAATAAGGATCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGATCCAAGCGTTATCCGGAATCATTGGGTTTAAAGGGTCCGTAGGCGGTCTTATAAGTCAGTGGTGAAATCCCATCGCTCAACGATGGAACTGCCATTGATACTGTAAGACTTGAATACTTAGGAAGTAACTAGAATATGTAGTGTAGCGGTGAAATGCTTAGATATTACATGGAATACCAATTGCGAAGGCAGGTTACTACTAAGTGATTGACGCTGATGGACGAAAGCGTGGGGAGCGAACA</t>
-  </si>
-  <si>
-    <t>0872ee96003e931447bfbda18e048d00</t>
-  </si>
-  <si>
-    <t>TGGGGAATATTGGGCAATGGAGGAAACTCTGACCCAGCGACGCCGCGTGAGGGATGAAGGCCTTCGGGTTGTAAACCTCTTTCAGTAGGGAAGAAGCGAAAGTGACGGTACCTACAGAAGAAGCACCGGCTAACTATGTGCCAGCAGCCGCGGTAATACATAGGGTGCAAGCGTTGTCCGGAATTATTGGGCGTAAAGAGCTCGTAGGTGGTTCGATACGTCGGATGTGAAAATCAGGGGCTCAACCCCTGACCTGCATCCGATACGGTCGAGCTAGAGTTTGGTAGGGGAGACTGGAATTCCTGGTGTAGCGGTGGAATGCGCAGATATCAGGAGGAACACCGATGGCGAAGGCAGGTCTCTGGGCCAATACTGACACTGAGGAGCGAAAGCGTGGGGAGCGAACA</t>
-  </si>
-  <si>
-    <t>a1efbe23ef4d87a1d5684ac3e92d2bce</t>
-  </si>
-  <si>
-    <t>TGGGGAATATTGCGCAATGGGCGAAAGCCTGACGCAGCCATGCCGCGTGTGTGAAGAAGGCCTTCGGGTTGTAAAGCACTTTCAATTGGGAGGAAAGGTTCACGGTTAATAACCGTGAGCTGTGACGTTACCTTTAGAAGAAGCACCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGTGCGAGCGTTAATCGGAATTACTGGGCGTAAAGCGCGCGTAGGTGGTCTGTTAAGTCGGATGTGAAAGCCCCGGGCTCAACCTGGGAACTGCATTCGATACTGGCAGACTAGAGTGCGAGAGAGGGAGGTAGAATTCCATGTGTAGCGGTGAAATGCGTAGATATGTGGAGGAATACCAGTGGCGAAGGCGGCCTCCTGGCTCGACACTGACACTGAGGTGCGAAAGCGTGGGGAGCAAACA</t>
-  </si>
-  <si>
-    <t>Luminiphilus sp902623175</t>
-  </si>
-  <si>
-    <t>Halieaceae</t>
-  </si>
-  <si>
-    <t>Luminiphilus</t>
-  </si>
-  <si>
-    <t>sp902623175</t>
-  </si>
-  <si>
-    <t>fa45c880cabbeb9cc516c65edb6a81af</t>
-  </si>
-  <si>
-    <t>TGGGGAATCTTGCGCAATGGGCGAAAGCCTGACGCAGCAACGCCGCGTGCGGGATGAAGGCCTTCGGGTTGTAAACCGCTTTTAACAGGAACGAAAATGACGGTACCTGTAGAATAAGGTGCGGCCAACTACGTGCCAGCAGCCGCGGTGACACGTAGGCACCAAGCGTTGTCCGGATTTATTGGGCGTAAAGAGCTCGTAGGCGGTTCAGTAAGTCGGGTGTGAAAACTCTGGGCTTAACCCAGAGACGCCACTCGATACTACTGTGACTAGAGTTCGGTAGGGGAGCGGGGAATTCCTAGTGTAGCGGTGAAATGCGCAGATATTAGGAGGAACACCGGTGGCGAAGGCGCCGCTCTGGGCCGATACTGACGCTGAGGAGCGAAAGCGTGGGTAGCAAACA</t>
-  </si>
-  <si>
-    <t>Casp-actino8 sp016871395</t>
-  </si>
-  <si>
-    <t>Casp-actino8</t>
-  </si>
-  <si>
-    <t>sp016871395</t>
-  </si>
-  <si>
-    <t>d7a78db14cbb0629842daa8b8f45be2c</t>
-  </si>
-  <si>
-    <t>TGGGGAATATTGGGCAATGGAGGAAACTCTGACCCAGCGACGCCGCGTGAGGGATGAAGGCCTTCGGGTTGTAAACCTCTTTCAGTAGGGAAGAAGCGAAAGTGACGGTACCTACAGAAGAAGCACCGGCTAACTATGTGCCAGCAGCCGCGGTAATACATAGGGTGCAAGCGTTGTCCGGAATTATTGGGCGTAAAGAGCTCGTAGGTGGTTCGATACGTCGGATGTGAAAATCAGGGGCTCAACCCCTGACCTGCATCCGATACGGTCGAGCTGGAGTTTGGTAGGGGAGACTGGAATTCCTGGTGTAGCGGTGGAATGCGCAGATATCAGGAGGAACACCGATGGCGAAGGCAGGTCTCTGGGCCAATACTGACACTGAGGAGCGAAAGCGTGGGGAGCGAACA</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="378">
+  <si>
+    <t xml:space="preserve">datasetID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datasetName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filename</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bioatlas_resource_uid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ipt_resource_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBDI-ASV-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16S data from: Diversity of Pico- to Mesoplankton along the 2000 km Salinity Gradient of the Baltic Sea (Hu et al. 2016)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jane.doe@univ.se_210902-212121_ampliseq.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eventID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">institutionCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">institutionID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">collectionCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">materialSampleID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">associatedSequences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fieldNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">catalogNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">references</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eventDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">samplingProtocol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locationID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decimalLatitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decimalLongitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geodeticDatum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coordinateUncertaintyInMeters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dataGeneralizations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recordedBy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">municipality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verbatimLocality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumElevationInMeters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maximumElevationInMeters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimumDepthInMeters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maximumDepthInMeters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16S_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ror.org/026vcq606</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ebi.ac.uk/ena/browser/view/SAMEA3724531</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ebi.ac.uk/ena/browser/view/ERR1202034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some-catalogue-no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-07-13T07:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200–500 mL seawater were filtered onto 0.22 μm pore-size mixed cellulose ester membrane filters; https://doi.org/10.3389/fmicb.2016.00679</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPSG:4326</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coordinates generalized from original GPS coordinates to three decimals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arkona Basin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16S_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ebi.ac.uk/ena/browser/view/SAMEA3724535</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ebi.ac.uk/ena/browser/view/ERR1202038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-07-13T09:38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baltic Proper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16S_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ebi.ac.uk/ena/browser/view/SAMEA3724536</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ebi.ac.uk/ena/browser/view/ERR1202039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-07-13T13:55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">target_gene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">target_subfragment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lib_layout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seq_meth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pcr_primer_name_forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pcr_primer_name_reverse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pcr_primer_forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pcr_primer_reverse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denoising_appr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">env_broad_scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">env_local_scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">env_medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.3389/fmicb.2016.00679</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16S rRNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V3-V4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Illumina MiSeq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">341F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">805R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCTACGGGNGGCWGCAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GACTACHVGGGTATCTAATCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DADA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aquatic biome [ENVO:00002030]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marine biome [ENVO:00000447]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brackish water [ENVO:00002019]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measurementType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measurementTypeID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measurementValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measurementValueID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measurementUnit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measurementUnitID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measurementAccuracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measurementDeterminedDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measurementDeterminedBy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measurementMethod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measurementRemarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">salinity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">°C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asv_id_alias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNA_sequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">919a2aa9d306e4cf3fa9ca02a2aa5730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCGAGAATTTTTCACAATGGGGGAAACCCTGATGGAGCGACGCCGCGTGGAGGATGAAGGTTTTCGGATTGTAAACTCCTGTCATTAGAGAACAAGGCACATGGTTTAACTGGCCGTGTGTTGATAGTATCTGAAGAGGAAGGGACGGCTAACTCTGTGCCAGCAGCCGCGGTAATACAGAGGTCTCAAGCGTTGTTCGGATTCATTGGGCGTAAAGGGTGCGTAGGTGGCGAGGTAAGTCGGATGTGAAATCTCCAAGCTCAACTTGGAAACTGCATTCGATACTGCTTTGCTAGAGGATTGTAGAGGGCATTGGAATTCACGGTGTAGCAGTGAAATGCGTAGATATCGTGAGGAAGACCAGTGGCGAAGGCGAATGCCTGGGCAATTCCTGACACTGAGGCACGAAGGCCAGGGGAGCAAACG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1ead98754d34073a4606f7ff1e94126e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATTTTCCGCAATGGGCGCAAGCCTGACGGAGCAACGCCGCGTGAGGGATGAAGGCCTCTGGGCTGTAAACCTCTTTTATCAAGGAAGAAGATCTGACGGTACTTGATGAATAAGCCACGGCTAATTCCGTGCCAGCAGCCGCGGTAATACGGGAGTGGCAAGCGTTATCCGGAATTATTGGGCGTAAAGCGTCCGCAGGCGGTTTTACAAGTCTGTCGTTAAAACGTGGAGCTCAACTCCATTTCGGCGATGGAAACTGTAAGACTAGAGTGTGGTAGGGGCAGAGGGAATTCCCGGTGTAGCGGTGAAATGCGTAGATATCGGGAAGAACACCAGTGGCGAAGGCGCTCTGCTGGGCCATAACTGACGCTCATGGACGAAAGCTAGGGGAGCGAAAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43e088977eba5732bfa45e20b1d8cdd2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCGAGAATTTTTCACAATGGGGGAAACCCTGATGGAGCGACGCCGCGTGGAGGATGAAGGTTTTCGGATCGTAAACTCCTGTCATTAGAGAACAAGGCACACGGTTTAACTGGCTGTGTGTTGATAGTATCTGAAGAGGAAGGGACGGCTAACTCTGTGCCAGCAGCCGCGGTAATACAGAGGTCTCAAGCGTTGTTCGGATTCATTGGGCGTAAAGGGTGCGTAGGTGGCGAGGTAAGTCGGATGTGAAATCTCCAAGCTCAACTTGGAAACTGCATTCGATACTGCTTTGCTAGAGGATTGTAGAGGGCATTGGAATTCACGGTGTAGCAGTGAAATGCGTAGATATCGTGAGGAAGACCAGTGGCGAAGGCGAATGCCTGGGCAATTCCTGACACTGAGGCACGAAGGCCAGGGGAGCAAACG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1b2c41577c16f4c672a2a861e6b89b14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAGGGAATATTGGGCAATGGGCGAAAGCCTGACCCAGCGACGCCGCGTGAGGGATGAAGGTCTTCGGATTGTAAACCTCTTTCAGTAGGGAAGAAGCGAAAGTGACGGTACCTAAAGAAGAAGCACCGGCTAACTATGTGCCAGCAGCCGCGGTAATACATAGGGTGCAAGCGTTGTCCGGAATTATTGGGCGTAAAGAGCTCGTAGGTCGTTTGTCGCGTCGATTGTGAAAATCTGAGGCTCAACCTCAGACCTGCAGTCGATACGGGCAAACTAGAGTGTGGTAGGGGAGACTGGAATTCCTGGTGTAGCGGTGGAATGCGCAGATATCAGGAGGAACACCAATGGCGAAGGCAGGTCTCTGGGCCATAACTGACACTGAGGAGCGAAAGTGCGGGGAGCGAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40b37890b1b1fcdf0ece91f1da34c1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATTTTCCGCAATGGGCGCAAGCCTGACGGAGCAACGCCGCGTGAGGGATGAAGGCCTCTGGGCTGTAAACCTCTTTTATCAAGGAAGAAGATCTGACGGTACTTGATGAATAAGCCACGGCTAATTCCGTGCCAGCAGCCGCGGTAATACGGGAGTGGCAAGCGTTATCCGGAATTATTGGGCGTAAAGCGTCCGCAGGCGGTCTTGAAAGTCTGTTGTTAAAGCGTGGAGCTCAACTCCATTTCAGCAATGGAAACTAGAAGACTAGAGTGTGGTAGGGGCAGAGGGAATTCCCGGTGTAGCGGTGAAATGCGTAGATATCGGGAAGAACACCAGTGGCGAAGGCGCTCTGCTGGGCCATAACTGACGCTCATGGACGAAAGCCAGGGGAGCGAAAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ae71bf7c99d3583a2d8841e5911c5716</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATATTGGGCAATGGAGGAAACTCTGACCCAGCGACGCCGCGTGCGGGATGAAGGCCTTCGGGTTGTAAACCGCTTTCAGTAGGGAAGAAGCGAAAGTGACGGTACCTACAAAAGAAGCACCGGCTAACTATGTGCCAGCAGCCGCGGTAATACATAGGGTGCAAGCGTTGTCCGGAATTATTGGGCGTAAAGAGCTCGTAGGTCGTTTGTTACGTCGGATGTGAAAACCTGAGGCTCAACCTCAGGCCTGCATTCGATACGGGCAAACTAGAGTTTGGTAGGGGAGACTGGAATTCCTGGTGTAGCGGTGGAATGCGCAGATATCAGGAGGAACACCAATGGCGAAGGCAGGTCTCTGGGCCAATACTGACACTGAGGAGCGAAAGTCTGGGGAGCGAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">887bc7033b46d960e893caceb711700b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATCTTGCGCAATGGGCGAAAGCCTGACGCAGCAACGCCGCGTGCGGGAAGAAGGCTTTCGGGCTGTAAACCGCTTTCAGCAGGAACGAAAATGACGGTACCTGCAGAAGAAGGAGCGGCCAACTATGTGCCAGCAGCCGCGGTGATACATAGGCTTCAAGCGTTGTCCGGATTTATTGGGCGTAAAGAGTTCGTAGGCGGTCGAGTAAGTCGGGTGTGAAAATTCTGGGCTCAACCCAGAGACGCCACCCGATACTGCTTAACTTGAGTTCGATAGGGGAGTGGGGAATTCCTAGTGTAGCGGTGAAATGCGCAGATATTAGGAGGAACACCGGTGGCGAAGGCGCCACTCTGGATCGACACTGACGCTGAGGAACGAAAGCATGGGTAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88b5b5240649749ca876d10823045b01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATCTTGCGCAATGGGCGAAAGCCTGACGCAGCAACGCCGCGTGCGGGATGAAGGCCTTCGGGCTGTAAACCGCTTTCAGCAGGAACGAAAATGACGGTACCTGCAGAAGAAGGAGCGGCCAACTACGTGCCAGCAGCCGCGGTGACACGTAGGCTCCAAGCGTTGTCCGGATTTATTGGGCGTAAAGAGCTCGTAGGCGGTTGAGTAAGTCGGGTGTGAAAACTCTGGGCTTAACCCGGAGACGCCATCCGATACTGCTCTGACTAGAGTTCAGGAGGGGAGTGGGGAATTCCTAGTGTAGCGGTGAAATGCGCAGATATTAGGAGGAACACCGGTGGCGAAGGCGCCACTCTGGACTGAAACTGACGCTGAGGAGCGAAAGCATGGGTAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">95efad17b5fb6b91274a6ef3c47a098a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATTTTCCGCAATGGGCGCAAGCCTGACGGAGCAACGCCGCGTGAGGGATGAAGGCCTCTGGGCTGTAAACCTCTTTTATCAAGGAAGAAGATCTGACGGTACTTGATGAATAAGCCACGGCTAATTCCGTGCCAGCAGCCGCGGTAATACGGGAGTGGCAAGCGTTATCCGGAATTATTGGGCGTAAAGCGTCCGCAGGCGGTTTTACAAGTCTGTCGTTAAAACGTGGAGCTCAACTCCATTTCGGCGATGGAAACTGTAAGACTAGAGTGTGGTAGGGGCAGAGGGAATTCCCGGTGTAGCGGTGAAATGCGTAGATATCGGGAAGAACACCAGTGGCGAAGGCGCTCTGCTGGGCCATAACTGACGCTCATGGACGAAAGCCAGGGGAGCGAAAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c366064866eaed18a54d15640272ab34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATATTGGGCAATGGAGGAAACTCTGACCCAGCGACGCCGCGTGCGGGATGAAGGCCTTCGGGTTGTAAACCGCTTTCAGCAGGGAAGAAGCGAAAGTGACGGTACCTGCAGAAGAAGCACCGGCTAACTATGTGCCAGCAGCCGCGGTAATACATAGGGTGCAAGCGTTGTCCGGAATTATTGGGCGTAAAGAGCTCGTAGGTGGTTCGTCACGTCGGATGTGAAACTCTGGGGCTTAACCCCAGACCTGCATTCGATACGGGCGAGCTTGAGTATGGTAGGGGAGTCTGGAATTCCTGGTGTAGCGGTGGAATGCGCAGATATCAGGAGGAACACCAATGGCGAAGGCAGGACTCTGGGCCATTACTGACACTGAGGAGCGAAAGCGTGGGGAGCGAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">previous_identifications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">organism_quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacteria|Verrucomicrobiota|Verrucomicrobiae|Chthoniobacterales|UBA6821|UBA6821|||</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://plutof.ut.ee/#/sequence/view/0000X0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacteria|Cyanobacteria|Cyanobacteriia|PCC-6307|Cyanobiaceae|Synechococcus_D|||</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://plutof.ut.ee/#/sequence/view/0000X1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacteria|Verrucomicrobiota|Verrucomicrobiae|Chthoniobacterales|||||</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://plutof.ut.ee/#/sequence/view/0000X2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacteria|Actinobacteriota|Actinomycetia|Nanopelagicales|Nanopelagicaceae|Nanopelagicus|||</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://plutof.ut.ee/#/sequence/view/0000X3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacteria|Cyanobacteria|Cyanobacteriia|PCC-6307|Cyanobiaceae|UBA5018|||</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://plutof.ut.ee/#/sequence/view/0000X4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://plutof.ut.ee/#/sequence/view/0000X5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacteria|Actinobacteriota|Acidimicrobiia|Acidimicrobiales|Ilumatobacteraceae|BACL27|sp014190055||</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://plutof.ut.ee/#/sequence/view/0000X6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacteria|Actinobacteriota|Acidimicrobiia|Acidimicrobiales|Ilumatobacteraceae|UBA3006|||</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://plutof.ut.ee/#/sequence/view/0000X7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacteria|Cyanobacteria|Cyanobacteriia|PCC-6307|Cyanobiaceae||||</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://plutof.ut.ee/#/sequence/view/0000X8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacteria|Actinobacteriota|Actinomycetia|Nanopelagicales|Nanopelagicaceae|Planktophila|||</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://plutof.ut.ee/#/sequence/view/0000X9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asv_sequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scientificName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taxonRank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phylum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specificEpithet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infraspecificEpithet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">otu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">annotation_confidence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_identified</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reference_db</t>
+  </si>
+  <si>
+    <t xml:space="preserve">annotation_algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">identification_references</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taxon_remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">annotation_target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">target_criteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">target_prediction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JACTMZ01 sp018402585</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verrucomicrobiota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verrucomicrobiae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chthoniobacterales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JACTMZ01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp018402585</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBDI-GTDB-R07-RS207-1 (https://scilifelab.figshare.com/articles/dataset/SBDI_Sativa_curated_16S_GTDB_database/14869077/4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ampliseq v2.5.0 (https://nf-co.re/ampliseq) DADA2:assignTaxonomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.biodiversitydata.se/analyse-data/molecular-tools/#taxonomy-annotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domain = 'Bacteria'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assigned kingdom OR barrnap-positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyanobiaceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyanobacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyanobacteriia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCC-6307</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">MAG-120802 sp003569145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actinobacteriota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actinomycetia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nanopelagicales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nanopelagicaceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAG-120802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp003569145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ampliseq v2.5.0 (https://nf-co.re/ampliseq) DADA2:assignTaxonomy:addSpecies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyanobium_A sp015840335</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyanobium_A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp015840335</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nanopelagicus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BACL27 sp014190055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acidimicrobiia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acidimicrobiales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ilumatobacteraceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BACL27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp014190055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBA3006 sp002367695</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBA3006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp002367695</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planktophila sp015660815</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planktophila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp015660815</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7ff490fff9504446139943d9c4f1be4a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATCTTGCGCAATGGGCGAAAGCCTGACGCAGCAACGCCGCGTGCGGGATGAAGGCCTTCGGGTTGTAAACCGCTTTCAGCAGGAACGAAAATGACGGTACCTGCAGAAGAAGGAGCGGCCAACTACGTGCCAGCAGCCGCGGTGACACGTAGGCTCCAAGCGTTGTCCGGATTTATTGGGCGTAAAGAGCTCGTAGGCGGTTTAGTAAGTCGGGTGTTAAAACTCTGGGCTCAACCCGGAGACGCCATCCGATACTACTATGACTTGAGTTCAGGAGGGGAGCGGGGAATTCCTAGTGTAGCGGTGAAATGCGCAGATATTAGGAGGAACACCGGTGGCGAAGGCGCCGCTCTGGACTGAAACTGACGCTGAGGAGCGAAAGCATGGGTAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96ff11f3fbe3bfe47f11753d3615eff9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAAGGAATATTGGGCAATGGACGCAAGTCTGACCCAGCCATCCCGCGTGCAGGACGAATGCCCTATGGGTTGTAAACTGCTTTTGTTTGGGAAGAAATGTATTCTTTTAAGAGTATTTGACGGTACCAGACGAATAAGCACCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGTGCAAGCGTTATCCGGAATCACTGGGTTTAAAGGGTGCGTAGGCGGCCAGATAAGTCAGAGGTGAAAGTTTCCGGCTCAACCGGGAGATTGCCTTTGATACTGTTTGGCTTGAATCAGATTGAGGTTGGCGGAATGTGACATGTAGCGGTGAAATGCATAGATATGTCATAGAACATCGATTGCGAAGGCAGCTGGCTGGATCTGTATTGACGCTGAGGCACGAAAGCGTGGGGAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saprospiraceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacteroidota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacteroidia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chitinophagales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60c5874530fb102c40f246e7b59cad1b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAGGGAATCTTAGACAATGGGGGCAACCCTGATCTAGCCATGCCGCGTGTGTGATGAAGGCCCTAGGGTCGTAAAGCACTTTCGCCAGAGATGATAATGACAGTATCTGGTAAAGAAACCCCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGGGTTAGCGTTGTTCGGAATTACTGGGCGTAAAGCGCACGTAGGCGGATTAGTAAGTTAGAGGTGAAATCCCAGGGCTCAACCCTGGAACTGCCTTTAATACTGCTAGTCTTGAGTTCGAGAGAGGTAAGTGGAATTCCGAGTGTAGAGGTGAAATTCGTAGATATTCGGAGGAACACCAGTGGCGAAGGCGGCTTACTGGCTCGATACTGACGCTGAGGTGCGAAAGTGTGGGGAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planktomarina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proteobacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alphaproteobacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rhodobacterales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rhodobacteraceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cb8818c331eb97f13778cef034bb3af0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATCTTGCACAATGGGCGAAAGCCTGATGCAGCGATGCCGCGTGAGTGAAGAAGGCCTTTGGGTTGTAAAGCTCTTTTGTCGGGAAAGATAATGACTGTACCCGAAGAATAAGGTCCGGCTAACTTCGTGCCAGCAGCCGCGGTAATACGAAGGGACCTAGCGTAGTTCGGAATTACTGGGCGTAAAGAGTATGTAGGCGGCTAGATAAGTTAATTGTGAAAGCCCAAAGCTTAACTTTGGAATTGCAATTAAAACTATTTAGCTGGAGTATGATAGAGGAAAGCGGAATACATAGTGTAGAGGTGAAATTCGTAGATATTATGTAGAACACCAGTTGCGAAGGCGGCTTTCTGGATCATTACTGACGCTGAGATACGAAAGTATGGGTAGCGAAGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMCC9063 sp000750175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pelagibacterales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pelagibacteraceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMCC9063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp000750175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53964bef6e413d0037100ef13b369504</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCGAGAATCTTCGGCAATGGGCGAAAGCCTGACCGAGCGATGCCGCGTGCGGGATGAAGGCCCTCGGGTTGTAAACCGCTGTCAACGAGGAGGAAGTGCAAGGGGGTTCTCCCTTTTGTTTGACCTATTCGAGAAGGAAGTACGGGCTAAGTTCGTGCCAGCAGCCGCGGTAAGACGAACCGTACAAACGTTATTCGGAATTATTGGGCTTAAAGGGTGCGTAGGCTGCGCGGAAAGTTGGGTGTGAAAGCCCTCGGCTCAACCGAGGAATTGCGCCCAAAACTACCGTGCTCGAGGGAGACAGAGGTGAGCGGAACTCAAGGTGGAGCGGTGAAATGCGTTGATATCTTGAGGAACACCGGTGGCGAAAGCGGCTCACTGGGTCTCTTCTGACGCTGAGGCACGAAAGCCAAGGTAGCAAACG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M30B53 sp018401745</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planctomycetota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planctomycetia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pirellulales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBA1268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M30B53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp018401745</t>
+  </si>
+  <si>
+    <t xml:space="preserve">766533668513f1de8efb46206dd0e235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATTTTCCGCAATGGGCGAAAGCCTGACGGAGCAACGCCGCGTGAGGGATGAAGGCCTCTGGGCTGTAAACCTCTTTTATCAAGGAAGAAGATCTGACGGTACTTGATGAATAAGCCACGGCTAATTCCGTGCCAGCAGCCGCGGTAATACGGGAGTGGCAAGCGTTATCCGGAATTATTGGGCGTAAAGCGTCCGCAGGCGGCCCAACAAGTCTGCTGTTAAAAAGTGGAGCTTAACTCCATCATGGCAGTGGAAACTGTTGGGCTAGAGTGTGGTAGGGGCAGAGGGAATTCCCGGTGTAGCGGTGAAATGCGTAGATATCGGGAAGAACACCAGTGGCGAAGGCGCTCTGCTGGGCCATCACTGACGCTCATGGACGAAAGCCAGGGGAGCGAAAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synechococcus_C sp014279835</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synechococcus_C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp014279835</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cac37e39df2461953f24398212940edf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGAGGAATATTGGACAATGGGCGAGAGCCTGATCCAGCCATGCCGCGTGCAGGAAGACTGCCCTATGGGTTGTAAACTGCTTTTATACAGGAAGAATAAGCCTTACGTGTAAGGTGATGACGGTACTGTAAGAATAAGGACCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGTCCGAGCGTTATCCGGAATTATTGGGTTTAAAGGGTCCGTAGGCGGATGATTAAGTCAGGGGTGAAAGTTTGCAGCTCAACTGTAAAATTGCCTTTGATACTGGTCATCTTGAGTTGTATTGAAGTAGGCGGAATATGTAGTGTAGCGGTGAAATGCATAGATATTACATAGAACACCAATTGCGAAGGCAGCTTACTAAGTACTAACTGACGCTGATGGACGAAAGCGTGGGTAGCGAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAG-120531 sp000173115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flavobacteriales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flavobacteriaceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAG-120531</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp000173115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73ec397d035244c7734fc7513050637d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATCTTGTGCAATGGACGAAAGTCTGACACAGCCACGCCGCGTGCGGGAAGAAGGCCTTCGGGTTGTAAACCGCTTTCAGCAGGAACGAAAATGACGGTACCTGCAGAAGAAGGAGCGGCCAACTACGTGCCAGCAGCCGCGGTGACACGTAGGCTCCAAGCGTTGTCCGGATTTATTGGGCGTAAAGAGCTCGTAGGCGGTTCAGCAAGTCGGGTGTGAAAACTCTGGGCTCAACCCAGAGCCTGCACCCGAAACTGCTGTGACTAGAGTTCGGTAGGGGAGTGGGGAATTCCTAGTGTAGCGGTGAAATGCGCAGATATTAGGAGGAACACCGATGGCGAAGGCACCACTCTGGGCCGAAACTGACGCTGAGGAGCGAAAGCGTGGGTAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBA2093 sp903929185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBA2093</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp903929185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d3a2fb3b65e96a6017a70182466040d8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAGGGAATATTGGGCAATGGTCGCAAGACTGACCCAGCCATGCCGCGTGCAGGAAGACGGCCCTCTGGGTTGTAAACTGCTTTTATCTGGGAAGAAAAAGTCCATGCGTGGAAAATTGCCGGTACCAGATGAATAAGCACCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGTGCAAGCGTTGTCCGGATTTATTGGGTTTAAAGGGTGCGTAGGCGGCTGAATAAGTCAGCGGTGAAAGACTTCGGCTTAACCGGAGCAGTGCCGTTGATACTGTTTAGCTTGAGTGTTGGAGGGGTACATGGAATTGATGGTGTAGCGGTGAAATGCATAGATACCATCAGGAACACCGATAGCGAAGGCATTGTACTGGCCAACAACTGACGCTGAGGCACGAAAGTGTGGGGATCGAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algoriphagus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cytophagales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyclobacteriaceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7208feb3afd481ebd51c04bb97e20644</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATCTTAGACAATGGGCGCAAGCCTGATCTAGCCATGCCGCGTGAGCGATGAAGGCCTTAGGGTTGTAAAGCTCTTTCAGTGGGGAAGATAATGACGGTACCCACAGAAGAAGCCCCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGGGCTAGCGTTGTTCGGAATTACTGGGCGTAAAGCGCGCGTAGGCGGATTGGAAAGTTGGAGGTGAAATCCCAGGGCTCAACCTTGGAACTGCCTTCAAAACTTCCAGTCTGGAGTTCGAGAGAGGTGAGTGGAATTCCGAGTGTAGAGGTGAAATTCGTAGATATTCGGAGGAACACCAGTGGCGAAGGCGGCTCACTGGCTCGATACTGACGCTGAGGTGCGAAAGCGTGGGGAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3451a03945f809e8f5d5a86e2d914717</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGAGGAATATTGGGCAATGGAGGCAACTCTGACCCAGCTATGCCGCGTGCAGGAAGACGGCCCTCTGGGTTGTAAACTGCTTTTGTTTGGGAATAAACCCTCCTACGTGTAGGAGGCTGAAGGTACCTTACGAATAAGCATCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGATGCAAGCGTTATCCGGATTTATTGGGTTTAAAGGGTCCGTAGGCGGATCTTTAAGTCAGTGGTGAAAGCCCACAGCTCAACTGTGGAACTGCCATTGATACTGGAGATCTTGAGTGTAGTAGAAGTAGGCGGAATAGGGCATGTAGCGGTGAAATGCATAGATATGCCCTAGAACACCGATTGCGAAGGCAGCTTACTATGTTACAACTGACGCTGAGGGACGAAAGCGTGGGGAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMED14 sp016868755</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schleiferiaceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMED14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp016868755</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f7600dd883bbcd817ee6cc47d0f7ee56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGAGGAATATTGGACAATGGGCGCAAGCCTGATCCAGCCATGCCGCGTGCAGGAAGACGGTCCTATGGATTGTAAACTGCTTTTATACAGGAAGAAACAACTCTACGTGTAGAGTCTTGACGGTACTGTAGGAATAAGGATCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGATCCAAGCGTTATCCGGAATCATTGGGTTTAAAGGGTCCGTAGGCGGTCTTATAAGTCAGTGGTGAAATCTCCTAGCTCAACTAGGAAACTGCCATTGATACTGTAAGACTTGAATTTTTGTGAAGTAACTAGAATATGTAGTGTAGCGGTGAAATGCTTAGATATTACATGGAATACCAATTGCGAAGGCAGGTTACTAACAAACGATTGACGCTGATGGACGAAAGCGTGGGGAGCGAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flavobacterium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eddec92462c6800adb4026d680198cb7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATTTTCCGCAATGGGCGAAAGCCTGACGGAGCAACGCCGCGTGAGGGATGAAGGCCTCTGGGCTGTAAACCTCTTTTATCAAGGAAGAAGATCTGACGGTACTTGATGAATAAGCCACGGCTAATTCCGTGCCAGCAGCCGCGGTAATACGGGAGTGGCAAGCGTTATCCGGAATTATTGGGCGTAAAGCGTCCGCAGGCGGCCCTTCAAGTCTGCTGTTAAAAAGTGGAGCTTAACTCCATCATGGCAGTGGAAACTGAGGGGCTTGAGTGTGGTAGGGGCAGAGGGAATTCCCGGTGTAGCGGTGAAATGCGTAGATATCGGGAAGAACACCAGTGGCGAAGGCGCTCTGCTGGGCCATCACTGACGCTCATGGACGAAAGCCAGGGGAGCGAAAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synechococcus_E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55060bfb51dc35530beac964e48e44bd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCGAGGATTTTTCTCAATGGGGGCAACCCTGAAGGAGCGACGCCGCGTGGAGGATGAAGGGCTTCGGCTCGTAAACTCCTGTCACCGACGAACAAGGCATCCGGATTAATAAATCGGATGCTTGATGGTAGTCGGAGAGGAAGGGGCGGCTAACTCTGTGCCAGCAGCCGCGGTGATACAGAGGCCCCAAGCGTTGTTCGGATTTACTGGGCGTAAAGGGTGTGTAGGGGGTCGGGTAAGTTTGACGTGAAATCCCGTTGCTCAACAACGGAACTGCGTCGAATACTGCTCGGCTGGAGGTTCGGAGATGAGGGCGGAATTCTCGGTGTAGCGGTGAAATGCGTAGATATCGAGAGGAACGCCGACGGCGAAAGCAGCCCTCAAGACGAAATCTGACCCTGAAACACGAAGGCCAGGGGAGCAAACG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBA3015 sp001438005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methylacidiphilales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBA3015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp001438005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9ac1d376f84dff0b4a0b11b609620bfa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATCTTAGACAATGGGCGCAAGCCTGATCTAGCCATGCCGCGTGAGTGATGAAGGCCTTAGGGTCGTAAAGCTCTTTCGCCTGTGATGATAATGACAGTAGCAGGTAAAGAAACCCCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGGGTTAGCGTTGTTCGGAATTACTGGGCGTAAAGCGCACGTAGGCGGATTGGAAAGTTGGGGGTGAAATCCCGGGGCTCAACCCCGGAACTGCCTCCAAAACTATCAGTCTAGAGTTCGAGAGAGGTGAGTGGAATTCCAAGTGTAGAGGTGAAATTCGTAGATATTTGGAGGAACACCAGTGGCGAAGGCGGCTCACTGGCTCGATACTGACGCTGAGGTGCGAAAGTGTGGGGAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LGRT01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaf363d33b413559f355276afbb79f37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATCTTAGACAATGGGCGCAAGCCTGATCTAGCCATGCCGCGTGATCGATGAAGGCCTTAGGGTTGTAAAGATCTTTCAGTTGGGAAGATAATGACGGTACCAACAGAAGAAGCCCCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGGGCTAGCGTTATTCGGAATTACTGGGCGTAAAGCGCACGTAGGCGGATTAGAAAGTCAGAGGTGAAATCCCAGGGCTCAACCTTGGAACTGCCTTTGAAACTTCTAGTCTTGAGTTCGAGAGAGGTGAGTGGAATTCCGAGTGTAGAGGTGAAATTCGTAGATATTCGGAGGAACACCAGTGGCGAAGGCGGCTCACTGGCTCGATACTGACGCTGAGGTGCGAAAGCGTGGGGAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBA10365 sp003536295</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBA10365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp003536295</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19b76dc633050df9ec212f0995316cbd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATTTTGGACAATGGGCGAAAGCCTGATCCAGCAATGCCGCGTGTGCGAAGAAGGCCTTCGGGTTGTAAAGCACTTTTGTCAGGAAAGAAATTGTTCGGGCCAATACCCCGAGCCGTTGACGGTACCTGAAGAATAAGCACCGGCTAACTACGTGCCAGCAGCCGCGGTAATACGTAGGGTGCGAGCGTTAATCGGAATTACTGGGCGTAAAGCGTGCGCAGGCGGTTTGTTAAGACAGTTGTGAAATCCCCGGGCTCAACCTGGGAACTGCAATTGTGACTGGCAGGCTAGAGTTTGGCAGAGGGGGGTGGAATTCCTGGTGTAGCAGTGAAATGCGTAGATATCAGGAGGAACACCGATGGCGAAGGCAGCCCCCTGGGCCATGACTGACGCTCATGCACGAAAGCGTGGGGAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBA2463 sp018402635</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gammaproteobacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burkholderiales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burkholderiaceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBA2463</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp018402635</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3170f6094605a579e6a0e1fefd33a2a5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATCTTAGACAATGGGCGCAAGCCTGATCTAGCCATGCCGCGTGAGTGACGAAGGCCTTAGGGTCGTAAAGCTCTTTCGCCAGAGATGATAATGACAGTATCTGGTAAAGAAACCCCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGGGTTAGCGTTGTTCGGAATTACTGGGCGTAAAGCGCACGTAGGCGGATTGGAAAGTATGGGGTGAAATCCCAGGGCTCAACCCTGGAACGGCCTTGTAAACTCCCAGTCTAGAGTTCGAGAGAGGTGAGTGGAATTCCAAGTGTAGAGGTGAAATTCGTAGATATTTGGAGGAACACCAGTGGCGAAGGCGGCTCACTGGCTCGATACTGACGCTGAGGTGCGAAAGTGTGGGGAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yoonia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21bf8c2fc46ed6c2534c698b98cc683b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATTTTGGACAATGGGCGCAAGCCTGATCCAGCCATGCCGCGTGCAGGATGAAGGCCTTCGGGTTGTAAACTGCTTTTGTACGGAACGAAAAGGTTTGGCCTAATAAGCTGGACCCATGACGGTACCGTAAGAATAAGCACCGGCTAACTACGTGCCAGCAGCCGCGGTAATACGTAGGGTGCGAGCGTTAATCGGAATTACTGGGCGTAAAGCGTGCGCAGGCGGTTATGTAAGACAGATGTGAAATCCCCGGGCTCAACCTGGGAACTGCATTAGTGACTGCATAGCTGGAGTACGGCAGAGGGGGATGGAATTCCGCGTGTAGCAGTGAAATGCGTAGATATGCGGAGGAACACCGATGGCGAAGGCAATCCCCTGGGCCTGTACTGACGCTCATGCACGAAAGCGTGGGGAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curvibacter gracilis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curvibacter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gracilis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cc87cf7731ae4eb54c4d6a8169d4598e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATCTTGCGCAATGGGCGAAAGCCTGACGCAGCAACGCCGCGTGCGGGATGAAGGCCTTCGGGCTGTAAACCGCTTTCAGCAGGAACGAAAATGACGGTACCTGCAGAAGAAGGAGCGGCCAACTACGTGCCAGCAGCCGCGGTGACACGTAGGCTCCAAGCGTTGTCCGGATTTATTGGGCGTAAAGAGCTCGTAGGCGGTTTAGTAAGTCGGGTGTGAAAACTCTGGGCTTAACCCGGAGACGCCATCCGATACTGCTATGACTTGAGTTCAGGAGGGGAGCGGGGAATTCCTAGTGTAGCGGTGAAATGCGCAGATATTAGGAGGAACACCGGTGGCGAAGGCGCCGCTCTGGACTGAAACTGACGCTGAGGAGCGAAAGCATGGGTAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0aa4663de19d33cbaec31569d47cf191</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGAGGAATATTGGTCAATGGGCGCAAGCCTGAACCAGCCATGCCGCGTGCAGGAAGAATGCCCTATGGGTTGTAAACTGCTTTTATTTGGGAATAAACCTCTTTACGTGTAGAGAGCTGAAGGTACCAAATGAATAAGCACCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGTGCAAGCGTTATCCGGAATCATTGGGTTTAAAGGGTCCGCAGGCGGATTTATAAGTCAGTGGTGAAATCCTATCGCTTAACGATAGAACTGCCATTGATACTGTAAGTCTTGAATTCGGTCGGAGTGGGCGGAATGTGTAGTGTAGCGGTGAAATGCATAGATATTACACAGAACACCGATAGCGAAGGCAGCTCACTAGGCCTGAATTGACGCTCAGGGACGAAAGCGTGGGGATCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBA952 sp016872115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crocinitomicaceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBA952</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp016872115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ac4107604c179f2f8414333885255725</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATTTTCCGCAATGGGCGAAAGCCTGACGGAGCAATACCGCGTGAGGGAGGAAGGCTCTTGGGTTGTAAACCTCTTTTCTCAGGGAAGAACAGAATGACGGTACCTGAGGAATAAGCATCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGATGCAAGCGTTATCCGGAATGATTGGGCGTAAAGGGTCCGCAGGTGGCATTGTAAGTCTGCTGTTAAAGAGTTTGGCTCAACCAAATAAGAGCAGTGGAAACTACAAAGCTAGAGTGTGGTCGGGGCAGAGGGAATTCCTGGTGTAGCGGTGAAATGCGTAGATATCAGGAAGAACACCAGTGGCGAAGGCGCTCTGCTAGGCCGAGACTGACACTGAGGGACGAAAGCTAGGGGAGCGAATG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dolichospermum flosaquae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyanobacteriales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nostocaceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dolichospermum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flosaquae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">380d81417892576cb8aa4c50e92e5e1d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGAGGAATATTGGGCAATGGAGGCAACTCTGACCCAGCCATGCCGCGTGCAGGAATAAGGTCCTATGGATTGTAAACTGCTTTTATACAGGAAGAAACACTCGGACGTGTCCGAGCTTGACGGTACTGTATGAATAAGCACCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGTGCAAGCGTTATCCGGAATCATTGGGTTTAAAGGGTCCGCAGGCGGTCAATTAAGTCAGAGGTGAAATCCCATCGCTTAACGATGGAACTGCCTTTGATACTGGTTGACTTGAGTCATATGGAAGTAGATAGAATGTGTAGTGTAGCGGTGAAATGCATAGATATTACACAGAATACCGATTGCGAAGGCAGTCTACTACGTATGTACTGACGCTCATGGACGAAAGCGTGGGGAGCGAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polaribacter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b15dce65a0a29efb0bcfadedd72ede3c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATATTGGGCAATGGAGGGAACTCTGACCCAGCGACGCCGCGTGCGGGATGAAGGCCTTCGGGTTGTAAACCGCTTTCAGCAAGGAAGAAGCGAAAGTGACGGTACTTGCAGAAGAAGCACCGGCTAACTATGTGCCAGCAGCCGCGGTAATACATAGGGTGCAAGCGTTGTCCGGAATTATTGGGCGTAAAGAGCTCGTAGGTGGTTCGTCACGTCGGATGTGAAAATCTGGGGCTTAACCCCAGACCTGCATTCGATACGGGCGAGCTAGAGTGTGGTAGGGGAGACTGGAATTCCTGGTGTAGCGGTGGAATGCGCAGATATCAGGAGGAACACCAATGGCGAAGGCAGGTCTCTGGGCCATTACTGACACTGAGGAGCGAAAGCGTGGGGAGCGAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5d12a2cd51bf17060f60270529c5722e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATATTGGACAATGGGCGCAAGCCTGATCCAGCCATGCCGCGTGTGTGAAGAAGGCTCTAGGGTTGTAAAGCACTTTCAGTAGGGAGGAAGGCCAGAGTGTTAATAGCGCTTTGGATTGACGTTACCTACAGAAGCAGCACCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGTGCAAGCGTTAATCGGAATTACTGGGCGTAAAGCGCGCGTAGGCGGTTTGTTAAGTGTGATGTGAAAGCCCAGGGCTCAACCTTGGAACTGCATCACATACTGGCAAGCTAGAGTACGGTAGAGGGGGGTAGAATTCCATGTGTAGCGGTGAAATGCGTAGAGATGTGGAGGAATACCAGTGGCGAAGGCGGCCCCCTGGATCGATACTGACGCTGAGGTGCGAAAGCGTGGGGAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBA9145 sp001438145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pseudomonadales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pseudohongiellaceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBA9145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp001438145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ff9f5d078bc5ba693575630c8cdaef70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATTTTGGACAATGGGCGCAAGCCTGATCCAGCAATGCCGCGTGAGTGAAGAAGGCCTTCGGGTTGTAAAGCTCTTTTGTCAGGGAAGAAACGGTGAGAGCTAATATCTTTTGCTAATGACGGTACCTGAAGAATAAGCACCGGCTAACTACGTGCCAGCAGCCGCGGTAATACGTAGGGTGCAAGCGTTAATCGGAATTACTGGGCGTAAAGCGTGCGCAGGCGGTTATGTAAGACAGATGTGAAATGCCCGGGCTTAACCTGGGAACTGCATTTGTGACTGCATGGCTAGAGTGTGTCAGAGGGGGGTAGAATTCCACGTGTAGCAGTGAAATGCGTAGATATGTGGAGGAATACCGATGGCGAAGGCAGCCCCCTGGGATAACACTGACGCTCATGCACGAAAGCGTGGGGAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herbaspirillum sp004134995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herbaspirillum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp004134995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272f79649c2702bec9ff272552ffffcf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATTTTCCGCAATGGGCGAAAGCCTGACGGAGCAACGCCGCGTGAGGGATGAAGGCCTCTGGGCTGTAAACCTCTTTTATCAAGGAAGAAGATCTGACGGTACTTGATGAATAAGCCACGGCTAATTCCGTGCCAGCAGCCGCGGTAATACGGGAGTGGCAAGCGTTATCCGGAATTATTGGGCGTAAAGCGTCCGCAGGCGGTCTTGTAAGTCTGTCGTTAAAGCGTGGAGCTTAACTCCATTTCGGCGGTGGAAACTACAAGACTAGAGTGTGGTAGGGGCAGAGGGAATTCCCGGTGTAGCGGTGAAATGCGTAGATATCGGGAAGAACACCAGTGGCGAAGGCGCTCTGCTGGGCCATAACTGACGCTCATGGACGAAAGCCAGGGGAGCGAAAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7c11f640776d5482ec95173ca61de908</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATATTGCGCAATGGGCGAAAGCCTGACGCAGCAACGCCGCGTGAGGGATGACGGCCTTCGGGTTGTAAACCTCTTTCAGCAGGGAAGAAGCGAGAGTGACGGTACCTGCAGAAGAAGCACCGGCTAACTACGTGCCAGCAGCCGCGGTAATACGTAGGGTGCAAGCGTTGTCCGGATTTATTGGGCGTAAAGAGCTCGTAGGCGGTTAGTCGCGTCGGATGTGAAATCCTAGAGCTTAACTCTGGGCCTGCATTCGATACGGGCTGACTCGAGTATTGTAGGGGAGACTGGAACTCCTGGTGTAGCGGTGAAATGCGCAGATATCAGGAAGAACACCGGTGGCGAAGGCGGGTCTCTGGGCAATTACTGACGCTGAGGAGCGAAAGCGTGGGGAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S36-B12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfbb41fc686730dd0f3e13df27759598</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATCTTAGACAATGGGGGAAACCCTGATCTAGCCATGCCGCGTGAGTGACGAAGGCCTTAGGGTCGTAAAGCTCTTTCACCAGGGATGATAATGACAGTACCTGGAGAAGAAACCCCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGGGTTAGCGTTGTTCGGAATTACTGGGCGTAAAGCGCACGTAGGCGGATTAGTCAGTCAGAGGTGAAATCCCAGGGCTCAACCTTGGAACTGCCTTTGATACTGCTAGTCTTGAGTTCGAGAGAGGTGAGTGGAATTCCGAGTGTAGAGGTGAAATTCGTAGATATTCGGAGGAACACCAGTGGCGAAGGCGGCTCACTGGCTCGATACTGACGCTGAGGTGCGAAAGCGTGGGGAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roseicyclus sp015689735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roseicyclus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp015689735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1505e5de35661b77871b454a575c128a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCGAGAATAATTCACAATGGGGGCAACCCTGATGGTGCAACGCCGCGTGGAGGATGACGGTCTTCGGATTGTAAACTCCTGTCATCTGGGAGAAAGACCTGGCCGTTAATAGCGGACAGGGTTGATAGTACCAGAAGAGGAAGGGACGGCTAACTTCGTGCCAGCAGCCGCGGTAATACGAAGGTCCCAAGCGTTGTTCGGAATCACTGGGCGTAAAGGGAGCGTAGGCGGCGCGGTAAGTCAGATGTGAAATCCCGGGGCTCAACCCCGGAACTGCATCCGATACTGCCGTGCTTGAGCAATGGAGAGGTAGCTGGAATTATCGGTGTAGCAGTGAAATGCGTAGATATCGATAGGAACACTCGTGGCGAAAGCGAGCTACTGGACATTTGCTGACGCTGAGGCTCGAAGGCTAGGGGAGCGAAAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luteolibacter sp018402445</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verrucomicrobiales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akkermansiaceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luteolibacter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp018402445</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1424204d0b3becbb64ef0b61abb46473</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATTTTCCGCAATGGGCGCAAGCCTGACGGAGCAACGCCGCGTGAGGGACGAAGGCCTCTGGGCTGTAAACCTCTTTTCTCAAGGAAGAAGACATGACGGTACTTGAGGAATAAGCCACGGCTAATTCCGTGCCAGCAGCCGCGGTAATACGGGAGTGGCAAGCGTTATCCGGAATTATTGGGCGTAAAGCGTCCGCAGGCGGCCCAGCAAGTCTGTTGTTAAAAAGTGGAGCTCAACTCCATCCAGGCAATGGAAACTGCTGGGCTAGAGTGTGGTAGGGGCAGAGGGAATTCCCGGTGTAGCGGTGAAATGCGTAGATATCGGGAAGAACACCAGTGGCGAAGGCGCTCTGCTGGGCCATAACTGACGCTCATGGACGAAAGCCAGGGGAGCGAAAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MW101C3 sp002252635</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MW101C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp002252635</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a7e194b4ea4b1df360fce3d3770d58ee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATCTTGCGCAATGGGCGAAAGCCTGACGCAGCAACGCCGCGTGCGGGAAGAAGGCCTTAGGGTTGTAAACCGCTTTCAGCAGGGAAGAAAATGACTGTACCTGCAGAAGAAGGTGCGGCCAACTACGTGCCAGCAGCCGCGGTGACACGTAGGCACCAAGCGTTGTCCGGATTTATTGGGCGTAAAGAGCTCGTAGGCTGTTCAGTTAGTTGGGTGTGAAAACTCCGGGCTTAACCCGGAGCCGCCACCCAATACTGCTGTGACTAGAGTTCGGTAGGGGAGCGGGGAATTCCTAGTGTAGCGGTGAAATGCGCAGATATTAGGAGGAACACCGGTGGCGAAGGCGCCGCTCTGGGCCGAAACTGACGCTGAGGAGCGAAAGCATGGGTAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c750452151a7570b94c64f9fcb207d33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGAGGAATATTGGTCAATGGGCGCAAGCCTGAACCAGCCATGCCGCGTGCAGGAAGAATGCCCTATGGGTTGTAAACTGCTTTTATTTAGGAATAAACCTTTCTACGTGTAGAAAGCTGAAGGTACTGAATGAATAAGCACCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGTGCAAGCGTTATCCGGAATCATTGGGTTTAAAGGGTCCGCAGGCGGGCGTATAAGTCAGTGGTGAAATCCTGCAGCTTAACTGCAGAACTGCCATTGATACTGTACGTCTTGAATTCGGTCGAAGTGGGCGGAATGTGTAGTGTAGCGGTGAAATGCATAGATATTACACAGAACACCGATAGCGAAGGCAGCTCACTAGGCCTGGATTGACGCTCAGGGACGAAAGCGTGGGGATCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBA952 sp009926125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp009926125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">93185103563e99d5dbd1111548078ed7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATTTTGGACAATGGGCGAAAGCCTGATCCAGCCATTCCGCGTGCAGGATGAAGGCCCTCGGGTTGTAAACTGCTTTTGTACAGAACGAAAAGGTTTCTATTAATACTAGGAGCTCATGACGGTACTGTAAGAATAAGCACCGGCTAACTACGTGCCAGCAGCCGCGGTAATACGTAGGGTGCAAGCGTTAATCGGAATTACTGGGCGTAAAGCGTGCGCAGGCGGTTATATAAGTCAGATGTGAAATCCCCGGGCTCAACCTGGGAACTGCATTTGAGACTGTATAGCTAGAGTACGGTAGAGGGGGATGGAATTCCGCGTGTAGCAGTGAAATGCGTAGATATGCGGAGGAACACCGATGGCGAAGGCAATCCCCTGGACCTGTACTGACGCTCATGCACGAAAGCGTGGGGAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56fa1dafeb007219a436225686b03582</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCGAGGATTTTTCTCAATGGGGGCAACCCTGAAGGAGCGACGCCGCGTGGAGGATGAAGGGCTTCGGCTCGTAAACTCCTGTCACCGACGAACAAGGCATTCGGATTAATAAATCGGATGCTTGATGGTAGTCGGAGAGGAAGGGGCGGCTAACTCTGTGCCAGCAGCCGCGGTGATACAGAGGCCCCAAGCGTTGTTCGGATTTACTGGGCGTAAAGGGTGTGTAGGGGGTTGGGTAAGTTTGACGTGAAATCCCGTTGCTCAACAACGGAACTGCGTCGAATACTGCTCAGCTGGAGGTTCGGAGATGAGGGCGGAATTCTCGGTGTAGCGGTGAAATGCGTAGATATCGAGAGGAACGCCGATGGCGAAAGCAGCCCTCAAGACGAAATCTGACCCTGAAACACGAAGGCCAGGGGAGCAAACG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">458a614d9f091f772f92f51236d1105a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGAGGAATATTGGTCAATGGGCGCAAGCCTGAACCAGCCATGCCGCGTGCAGGAAGACGGTCCTATGGATTGTAAACTGCTTTTATACAGGAAGAAACCCTCCCACGTGTGGGAGATTGACGGTACTGTAGGAATAAGGATCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGATCCAAGCGTTATCCGGAATCATTGGGTTTAAAGGGTCCGTAGGCGGTCTTATAAGTCAGTGGTGAAATCCCATCGCTCAACGATGGAACTGCCATTGATACTGTAAGACTTGAATACTTAGGAAGTAACTAGAATATGTAGTGTAGCGGTGAAATGCTTAGATATTACATGGAATACCAATTGCGAAGGCAGGTTACTACTAAGTGATTGACGCTGATGGACGAAAGCGTGGGGAGCGAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0872ee96003e931447bfbda18e048d00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATATTGGGCAATGGAGGAAACTCTGACCCAGCGACGCCGCGTGAGGGATGAAGGCCTTCGGGTTGTAAACCTCTTTCAGTAGGGAAGAAGCGAAAGTGACGGTACCTACAGAAGAAGCACCGGCTAACTATGTGCCAGCAGCCGCGGTAATACATAGGGTGCAAGCGTTGTCCGGAATTATTGGGCGTAAAGAGCTCGTAGGTGGTTCGATACGTCGGATGTGAAAATCAGGGGCTCAACCCCTGACCTGCATCCGATACGGTCGAGCTAGAGTTTGGTAGGGGAGACTGGAATTCCTGGTGTAGCGGTGGAATGCGCAGATATCAGGAGGAACACCGATGGCGAAGGCAGGTCTCTGGGCCAATACTGACACTGAGGAGCGAAAGCGTGGGGAGCGAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a1efbe23ef4d87a1d5684ac3e92d2bce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATATTGCGCAATGGGCGAAAGCCTGACGCAGCCATGCCGCGTGTGTGAAGAAGGCCTTCGGGTTGTAAAGCACTTTCAATTGGGAGGAAAGGTTCACGGTTAATAACCGTGAGCTGTGACGTTACCTTTAGAAGAAGCACCGGCTAACTCCGTGCCAGCAGCCGCGGTAATACGGAGGGTGCGAGCGTTAATCGGAATTACTGGGCGTAAAGCGCGCGTAGGTGGTCTGTTAAGTCGGATGTGAAAGCCCCGGGCTCAACCTGGGAACTGCATTCGATACTGGCAGACTAGAGTGCGAGAGAGGGAGGTAGAATTCCATGTGTAGCGGTGAAATGCGTAGATATGTGGAGGAATACCAGTGGCGAAGGCGGCCTCCTGGCTCGACACTGACACTGAGGTGCGAAAGCGTGGGGAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luminiphilus sp902623175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halieaceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luminiphilus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp902623175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fa45c880cabbeb9cc516c65edb6a81af</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATCTTGCGCAATGGGCGAAAGCCTGACGCAGCAACGCCGCGTGCGGGATGAAGGCCTTCGGGTTGTAAACCGCTTTTAACAGGAACGAAAATGACGGTACCTGTAGAATAAGGTGCGGCCAACTACGTGCCAGCAGCCGCGGTGACACGTAGGCACCAAGCGTTGTCCGGATTTATTGGGCGTAAAGAGCTCGTAGGCGGTTCAGTAAGTCGGGTGTGAAAACTCTGGGCTTAACCCAGAGACGCCACTCGATACTACTGTGACTAGAGTTCGGTAGGGGAGCGGGGAATTCCTAGTGTAGCGGTGAAATGCGCAGATATTAGGAGGAACACCGGTGGCGAAGGCGCCGCTCTGGGCCGATACTGACGCTGAGGAGCGAAAGCGTGGGTAGCAAACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Casp-actino8 sp016871395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Casp-actino8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sp016871395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d7a78db14cbb0629842daa8b8f45be2c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TGGGGAATATTGGGCAATGGAGGAAACTCTGACCCAGCGACGCCGCGTGAGGGATGAAGGCCTTCGGGTTGTAAACCTCTTTCAGTAGGGAAGAAGCGAAAGTGACGGTACCTACAGAAGAAGCACCGGCTAACTATGTGCCAGCAGCCGCGGTAATACATAGGGTGCAAGCGTTGTCCGGAATTATTGGGCGTAAAGAGCTCGTAGGTGGTTCGATACGTCGGATGTGAAAATCAGGGGCTCAACCCCTGACCTGCATCCGATACGGTCGAGCTGGAGTTTGGTAGGGGAGACTGGAATTCCTGGTGTAGCGGTGGAATGCGCAGATATCAGGAGGAACACCGATGGCGAAGGCAGGTCTCTGGGCCAATACTGACACTGAGGAGCGAAAGCGTGGGGAGCGAACA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1181,7 +1171,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1206,21 +1195,12 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1502,19 +1482,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1531,7 +1506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1541,22 +1516,24 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
+      <c r="D2"/>
+      <c r="E2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Y4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1633,7 +1610,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1643,44 +1620,54 @@
       <c r="C2" t="s">
         <v>35</v>
       </c>
+      <c r="D2"/>
       <c r="E2" t="s">
         <v>36</v>
       </c>
       <c r="F2" t="s">
         <v>37</v>
       </c>
+      <c r="G2"/>
       <c r="H2" t="s">
         <v>38</v>
       </c>
+      <c r="I2"/>
       <c r="J2" t="s">
         <v>39</v>
       </c>
       <c r="K2" t="s">
         <v>40</v>
       </c>
-      <c r="M2">
-        <v>55.185000000000002</v>
-      </c>
-      <c r="N2">
+      <c r="L2"/>
+      <c r="M2" t="n">
+        <v>55.185</v>
+      </c>
+      <c r="N2" t="n">
         <v>13.791</v>
       </c>
       <c r="O2" t="s">
         <v>41</v>
       </c>
+      <c r="P2"/>
       <c r="Q2" t="s">
         <v>42</v>
       </c>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
       <c r="U2" t="s">
         <v>43</v>
       </c>
-      <c r="X2">
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2" t="n">
         <v>3</v>
       </c>
-      <c r="Y2">
+      <c r="Y2" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1690,44 +1677,54 @@
       <c r="C3" t="s">
         <v>35</v>
       </c>
+      <c r="D3"/>
       <c r="E3" t="s">
         <v>45</v>
       </c>
       <c r="F3" t="s">
         <v>46</v>
       </c>
+      <c r="G3"/>
       <c r="H3" t="s">
         <v>38</v>
       </c>
+      <c r="I3"/>
       <c r="J3" t="s">
         <v>47</v>
       </c>
       <c r="K3" t="s">
         <v>40</v>
       </c>
-      <c r="M3">
-        <v>55.433999999999997</v>
-      </c>
-      <c r="N3">
-        <v>14.813000000000001</v>
+      <c r="L3"/>
+      <c r="M3" t="n">
+        <v>55.434</v>
+      </c>
+      <c r="N3" t="n">
+        <v>14.813</v>
       </c>
       <c r="O3" t="s">
         <v>41</v>
       </c>
+      <c r="P3"/>
       <c r="Q3" t="s">
         <v>42</v>
       </c>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
       <c r="U3" t="s">
         <v>48</v>
       </c>
-      <c r="X3">
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3" t="n">
         <v>3</v>
       </c>
-      <c r="Y3">
+      <c r="Y3" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1737,58 +1734,68 @@
       <c r="C4" t="s">
         <v>35</v>
       </c>
+      <c r="D4"/>
       <c r="E4" t="s">
         <v>50</v>
       </c>
       <c r="F4" t="s">
         <v>51</v>
       </c>
+      <c r="G4"/>
       <c r="H4" t="s">
         <v>38</v>
       </c>
+      <c r="I4"/>
       <c r="J4" t="s">
         <v>52</v>
       </c>
       <c r="K4" t="s">
         <v>40</v>
       </c>
-      <c r="M4">
-        <v>56.031999999999996</v>
-      </c>
-      <c r="N4">
-        <v>16.649999999999999</v>
+      <c r="L4"/>
+      <c r="M4" t="n">
+        <v>56.032</v>
+      </c>
+      <c r="N4" t="n">
+        <v>16.65</v>
       </c>
       <c r="O4" t="s">
         <v>41</v>
       </c>
+      <c r="P4"/>
       <c r="Q4" t="s">
         <v>42</v>
       </c>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
       <c r="U4" t="s">
         <v>48</v>
       </c>
-      <c r="X4">
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4" t="n">
         <v>3</v>
       </c>
-      <c r="Y4">
+      <c r="Y4" t="n">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1832,7 +1839,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1876,7 +1883,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1920,7 +1927,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1966,19 +1973,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -2016,105 +2023,153 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>90</v>
       </c>
-      <c r="D2">
+      <c r="C2"/>
+      <c r="D2" t="n">
         <v>7.25</v>
       </c>
+      <c r="E2"/>
       <c r="F2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+    </row>
+    <row r="3">
       <c r="A3" t="s">
         <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="D3">
+      <c r="C3"/>
+      <c r="D3" t="n">
         <v>7.23</v>
       </c>
+      <c r="E3"/>
       <c r="F3" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
         <v>49</v>
       </c>
       <c r="B4" t="s">
         <v>90</v>
       </c>
-      <c r="D4">
+      <c r="C4"/>
+      <c r="D4" t="n">
         <v>6.97</v>
       </c>
+      <c r="E4"/>
       <c r="F4" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="D5">
-        <v>16.899999999999999</v>
-      </c>
+      <c r="C5"/>
+      <c r="D5" t="n">
+        <v>16.9</v>
+      </c>
+      <c r="E5"/>
       <c r="F5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+    </row>
+    <row r="6">
       <c r="A6" t="s">
         <v>44</v>
       </c>
       <c r="B6" t="s">
         <v>92</v>
       </c>
-      <c r="D6">
-        <v>17.399999999999999</v>
-      </c>
+      <c r="C6"/>
+      <c r="D6" t="n">
+        <v>17.4</v>
+      </c>
+      <c r="E6"/>
       <c r="F6" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+    </row>
+    <row r="7">
       <c r="A7" t="s">
         <v>49</v>
       </c>
       <c r="B7" t="s">
         <v>92</v>
       </c>
-      <c r="D7">
-        <v>16.899999999999999</v>
-      </c>
+      <c r="C7"/>
+      <c r="D7" t="n">
+        <v>16.9</v>
+      </c>
+      <c r="E7"/>
       <c r="F7" t="s">
         <v>93</v>
       </c>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>94</v>
       </c>
@@ -2122,7 +2177,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2130,7 +2185,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -2138,7 +2193,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -2146,7 +2201,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -2154,7 +2209,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -2162,7 +2217,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -2170,7 +2225,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -2178,7 +2233,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" t="s">
         <v>110</v>
       </c>
@@ -2186,7 +2241,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -2194,7 +2249,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -2204,19 +2259,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>94</v>
       </c>
@@ -2233,7 +2288,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2246,11 +2301,11 @@
       <c r="D2" t="s">
         <v>33</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>2235</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -2263,11 +2318,11 @@
       <c r="D3" t="s">
         <v>33</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>1033</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -2280,11 +2335,11 @@
       <c r="D4" t="s">
         <v>33</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>795</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -2297,11 +2352,11 @@
       <c r="D5" t="s">
         <v>33</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="n">
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -2314,11 +2369,11 @@
       <c r="D6" t="s">
         <v>33</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="n">
         <v>572</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -2331,11 +2386,11 @@
       <c r="D7" t="s">
         <v>33</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -2348,11 +2403,11 @@
       <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" t="s">
         <v>110</v>
       </c>
@@ -2365,11 +2420,11 @@
       <c r="D9" t="s">
         <v>33</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="n">
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -2382,11 +2437,11 @@
       <c r="D10" t="s">
         <v>33</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="n">
         <v>312</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -2399,11 +2454,11 @@
       <c r="D11" t="s">
         <v>33</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="n">
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -2416,11 +2471,11 @@
       <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="n">
         <v>16165</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -2433,11 +2488,11 @@
       <c r="D13" t="s">
         <v>44</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="n">
         <v>6836</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" t="s">
         <v>100</v>
       </c>
@@ -2450,11 +2505,11 @@
       <c r="D14" t="s">
         <v>44</v>
       </c>
-      <c r="E14">
+      <c r="E14" t="n">
         <v>4941</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" t="s">
         <v>102</v>
       </c>
@@ -2467,11 +2522,11 @@
       <c r="D15" t="s">
         <v>44</v>
       </c>
-      <c r="E15">
+      <c r="E15" t="n">
         <v>1187</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" t="s">
         <v>104</v>
       </c>
@@ -2484,11 +2539,11 @@
       <c r="D16" t="s">
         <v>44</v>
       </c>
-      <c r="E16">
+      <c r="E16" t="n">
         <v>2827</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" t="s">
         <v>106</v>
       </c>
@@ -2501,11 +2556,11 @@
       <c r="D17" t="s">
         <v>44</v>
       </c>
-      <c r="E17">
+      <c r="E17" t="n">
         <v>464</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" t="s">
         <v>108</v>
       </c>
@@ -2518,11 +2573,11 @@
       <c r="D18" t="s">
         <v>44</v>
       </c>
-      <c r="E18">
+      <c r="E18" t="n">
         <v>494</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" t="s">
         <v>110</v>
       </c>
@@ -2535,11 +2590,11 @@
       <c r="D19" t="s">
         <v>44</v>
       </c>
-      <c r="E19">
+      <c r="E19" t="n">
         <v>1641</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" t="s">
         <v>112</v>
       </c>
@@ -2552,11 +2607,11 @@
       <c r="D20" t="s">
         <v>44</v>
       </c>
-      <c r="E20">
+      <c r="E20" t="n">
         <v>1685</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" t="s">
         <v>114</v>
       </c>
@@ -2569,11 +2624,11 @@
       <c r="D21" t="s">
         <v>44</v>
       </c>
-      <c r="E21">
+      <c r="E21" t="n">
         <v>1436</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" t="s">
         <v>96</v>
       </c>
@@ -2586,11 +2641,11 @@
       <c r="D22" t="s">
         <v>49</v>
       </c>
-      <c r="E22">
+      <c r="E22" t="n">
         <v>12855</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" t="s">
         <v>98</v>
       </c>
@@ -2603,11 +2658,11 @@
       <c r="D23" t="s">
         <v>49</v>
       </c>
-      <c r="E23">
+      <c r="E23" t="n">
         <v>12742</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" t="s">
         <v>100</v>
       </c>
@@ -2620,11 +2675,11 @@
       <c r="D24" t="s">
         <v>49</v>
       </c>
-      <c r="E24">
+      <c r="E24" t="n">
         <v>3666</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" t="s">
         <v>102</v>
       </c>
@@ -2637,11 +2692,11 @@
       <c r="D25" t="s">
         <v>49</v>
       </c>
-      <c r="E25">
+      <c r="E25" t="n">
         <v>2307</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -2654,11 +2709,11 @@
       <c r="D26" t="s">
         <v>49</v>
       </c>
-      <c r="E26">
+      <c r="E26" t="n">
         <v>1513</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -2671,11 +2726,11 @@
       <c r="D27" t="s">
         <v>49</v>
       </c>
-      <c r="E27">
+      <c r="E27" t="n">
         <v>617</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -2688,11 +2743,11 @@
       <c r="D28" t="s">
         <v>49</v>
       </c>
-      <c r="E28">
+      <c r="E28" t="n">
         <v>839</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" t="s">
         <v>110</v>
       </c>
@@ -2705,11 +2760,11 @@
       <c r="D29" t="s">
         <v>49</v>
       </c>
-      <c r="E29">
+      <c r="E29" t="n">
         <v>2961</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -2722,11 +2777,11 @@
       <c r="D30" t="s">
         <v>49</v>
       </c>
-      <c r="E30">
+      <c r="E30" t="n">
         <v>1689</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -2739,25 +2794,25 @@
       <c r="D31" t="s">
         <v>49</v>
       </c>
-      <c r="E31">
+      <c r="E31" t="n">
         <v>2784</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:V51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>94</v>
       </c>
@@ -2825,7 +2880,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -2859,10 +2914,12 @@
       <c r="K2" t="s">
         <v>165</v>
       </c>
-      <c r="N2">
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2" t="n">
         <v>0.95</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P2" t="s">
@@ -2887,7 +2944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -2921,10 +2978,12 @@
       <c r="K3" t="s">
         <v>175</v>
       </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3" s="1">
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P3" t="s">
@@ -2949,7 +3008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -2983,10 +3042,12 @@
       <c r="K4" t="s">
         <v>165</v>
       </c>
-      <c r="N4">
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4" t="n">
         <v>0.86</v>
       </c>
-      <c r="O4" s="1">
+      <c r="O4" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P4" t="s">
@@ -3011,7 +3072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -3045,10 +3106,12 @@
       <c r="K5" t="s">
         <v>182</v>
       </c>
-      <c r="N5">
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5" t="n">
         <v>0.87</v>
       </c>
-      <c r="O5" s="1">
+      <c r="O5" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P5" t="s">
@@ -3073,7 +3136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -3107,10 +3170,12 @@
       <c r="K6" t="s">
         <v>186</v>
       </c>
-      <c r="N6">
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6" t="n">
         <v>0.96</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P6" t="s">
@@ -3135,7 +3200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -3169,10 +3234,12 @@
       <c r="K7" t="s">
         <v>175</v>
       </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7" s="1">
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P7" t="s">
@@ -3197,7 +3264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -3231,10 +3298,12 @@
       <c r="K8" t="s">
         <v>193</v>
       </c>
-      <c r="N8">
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8" t="n">
         <v>0.99</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P8" t="s">
@@ -3259,7 +3328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" t="s">
         <v>110</v>
       </c>
@@ -3293,10 +3362,12 @@
       <c r="K9" t="s">
         <v>196</v>
       </c>
-      <c r="N9">
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9" t="n">
         <v>0.93</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O9" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P9" t="s">
@@ -3321,7 +3392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -3355,10 +3426,12 @@
       <c r="K10" t="s">
         <v>175</v>
       </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="O10" s="1">
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O10" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P10" t="s">
@@ -3383,7 +3456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" t="s">
         <v>114</v>
       </c>
@@ -3417,10 +3490,12 @@
       <c r="K11" t="s">
         <v>199</v>
       </c>
-      <c r="N11">
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11" t="n">
         <v>0.77</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P11" t="s">
@@ -3445,7 +3520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" t="s">
         <v>200</v>
       </c>
@@ -3479,10 +3554,12 @@
       <c r="K12" t="s">
         <v>196</v>
       </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-      <c r="O12" s="1">
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P12" t="s">
@@ -3507,7 +3584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" t="s">
         <v>202</v>
       </c>
@@ -3541,10 +3618,12 @@
       <c r="K13" t="s">
         <v>175</v>
       </c>
-      <c r="N13">
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13" t="n">
         <v>0.99</v>
       </c>
-      <c r="O13" s="1">
+      <c r="O13" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P13" t="s">
@@ -3569,7 +3648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" t="s">
         <v>208</v>
       </c>
@@ -3603,10 +3682,12 @@
       <c r="K14" t="s">
         <v>175</v>
       </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-      <c r="O14" s="1">
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P14" t="s">
@@ -3631,7 +3712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" t="s">
         <v>215</v>
       </c>
@@ -3665,10 +3746,12 @@
       <c r="K15" t="s">
         <v>221</v>
       </c>
-      <c r="N15">
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15" t="n">
         <v>0.96</v>
       </c>
-      <c r="O15" s="1">
+      <c r="O15" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P15" t="s">
@@ -3693,7 +3776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" t="s">
         <v>222</v>
       </c>
@@ -3727,10 +3810,12 @@
       <c r="K16" t="s">
         <v>230</v>
       </c>
-      <c r="N16">
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16" t="n">
         <v>0.97</v>
       </c>
-      <c r="O16" s="1">
+      <c r="O16" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P16" t="s">
@@ -3755,7 +3840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" t="s">
         <v>231</v>
       </c>
@@ -3789,10 +3874,12 @@
       <c r="K17" t="s">
         <v>235</v>
       </c>
-      <c r="N17">
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17" t="n">
         <v>0.6</v>
       </c>
-      <c r="O17" s="1">
+      <c r="O17" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P17" t="s">
@@ -3817,7 +3904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" t="s">
         <v>236</v>
       </c>
@@ -3851,10 +3938,12 @@
       <c r="K18" t="s">
         <v>242</v>
       </c>
-      <c r="N18">
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18" t="n">
         <v>0.83</v>
       </c>
-      <c r="O18" s="1">
+      <c r="O18" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P18" t="s">
@@ -3879,7 +3968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" t="s">
         <v>243</v>
       </c>
@@ -3913,10 +4002,12 @@
       <c r="K19" t="s">
         <v>247</v>
       </c>
-      <c r="N19">
-        <v>1</v>
-      </c>
-      <c r="O19" s="1">
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19" t="n">
+        <v>1</v>
+      </c>
+      <c r="O19" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P19" t="s">
@@ -3941,7 +4032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" t="s">
         <v>248</v>
       </c>
@@ -3975,10 +4066,12 @@
       <c r="K20" t="s">
         <v>175</v>
       </c>
-      <c r="N20">
-        <v>1</v>
-      </c>
-      <c r="O20" s="1">
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O20" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P20" t="s">
@@ -4003,7 +4096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" t="s">
         <v>253</v>
       </c>
@@ -4037,10 +4130,12 @@
       <c r="K21" t="s">
         <v>175</v>
       </c>
-      <c r="N21">
-        <v>1</v>
-      </c>
-      <c r="O21" s="1">
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O21" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P21" t="s">
@@ -4065,7 +4160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" t="s">
         <v>255</v>
       </c>
@@ -4099,10 +4194,12 @@
       <c r="K22" t="s">
         <v>260</v>
       </c>
-      <c r="N22">
-        <v>1</v>
-      </c>
-      <c r="O22" s="1">
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22" t="n">
+        <v>1</v>
+      </c>
+      <c r="O22" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P22" t="s">
@@ -4127,7 +4224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" t="s">
         <v>261</v>
       </c>
@@ -4161,10 +4258,12 @@
       <c r="K23" t="s">
         <v>175</v>
       </c>
-      <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="O23" s="1">
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23" t="n">
+        <v>1</v>
+      </c>
+      <c r="O23" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P23" t="s">
@@ -4189,7 +4288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" t="s">
         <v>264</v>
       </c>
@@ -4223,10 +4322,12 @@
       <c r="K24" t="s">
         <v>175</v>
       </c>
-      <c r="N24">
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24" t="n">
         <v>0.96</v>
       </c>
-      <c r="O24" s="1">
+      <c r="O24" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P24" t="s">
@@ -4251,7 +4352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" t="s">
         <v>267</v>
       </c>
@@ -4285,10 +4386,12 @@
       <c r="K25" t="s">
         <v>272</v>
       </c>
-      <c r="N25">
-        <v>1</v>
-      </c>
-      <c r="O25" s="1">
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25" t="n">
+        <v>1</v>
+      </c>
+      <c r="O25" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P25" t="s">
@@ -4313,7 +4416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" t="s">
         <v>273</v>
       </c>
@@ -4347,10 +4450,12 @@
       <c r="K26" t="s">
         <v>175</v>
       </c>
-      <c r="N26">
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26" t="n">
         <v>0.97</v>
       </c>
-      <c r="O26" s="1">
+      <c r="O26" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P26" t="s">
@@ -4375,7 +4480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" t="s">
         <v>276</v>
       </c>
@@ -4409,10 +4514,12 @@
       <c r="K27" t="s">
         <v>280</v>
       </c>
-      <c r="N27">
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27" t="n">
         <v>0.94</v>
       </c>
-      <c r="O27" s="1">
+      <c r="O27" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P27" t="s">
@@ -4437,7 +4544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" t="s">
         <v>281</v>
       </c>
@@ -4471,10 +4578,12 @@
       <c r="K28" t="s">
         <v>288</v>
       </c>
-      <c r="N28">
-        <v>1</v>
-      </c>
-      <c r="O28" s="1">
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28" t="n">
+        <v>1</v>
+      </c>
+      <c r="O28" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P28" t="s">
@@ -4499,7 +4608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" t="s">
         <v>289</v>
       </c>
@@ -4533,10 +4642,12 @@
       <c r="K29" t="s">
         <v>175</v>
       </c>
-      <c r="N29">
-        <v>1</v>
-      </c>
-      <c r="O29" s="1">
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29" t="n">
+        <v>1</v>
+      </c>
+      <c r="O29" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P29" t="s">
@@ -4561,7 +4672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" t="s">
         <v>292</v>
       </c>
@@ -4595,10 +4706,12 @@
       <c r="K30" t="s">
         <v>296</v>
       </c>
-      <c r="N30">
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30" t="n">
         <v>0.88</v>
       </c>
-      <c r="O30" s="1">
+      <c r="O30" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P30" t="s">
@@ -4623,7 +4736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" t="s">
         <v>297</v>
       </c>
@@ -4657,10 +4770,12 @@
       <c r="K31" t="s">
         <v>196</v>
       </c>
-      <c r="N31">
-        <v>1</v>
-      </c>
-      <c r="O31" s="1">
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31" t="n">
+        <v>1</v>
+      </c>
+      <c r="O31" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P31" t="s">
@@ -4685,7 +4800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" t="s">
         <v>299</v>
       </c>
@@ -4719,10 +4834,12 @@
       <c r="K32" t="s">
         <v>304</v>
       </c>
-      <c r="N32">
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32" t="n">
         <v>0.67</v>
       </c>
-      <c r="O32" s="1">
+      <c r="O32" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P32" t="s">
@@ -4747,7 +4864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="33">
       <c r="A33" t="s">
         <v>305</v>
       </c>
@@ -4781,10 +4898,12 @@
       <c r="K33" t="s">
         <v>311</v>
       </c>
-      <c r="N33">
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33" t="n">
         <v>0.96</v>
       </c>
-      <c r="O33" s="1">
+      <c r="O33" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P33" t="s">
@@ -4809,7 +4928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="34">
       <c r="A34" t="s">
         <v>312</v>
       </c>
@@ -4843,10 +4962,12 @@
       <c r="K34" t="s">
         <v>175</v>
       </c>
-      <c r="N34">
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34" t="n">
         <v>0.98</v>
       </c>
-      <c r="O34" s="1">
+      <c r="O34" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P34" t="s">
@@ -4871,7 +4992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="35">
       <c r="A35" t="s">
         <v>315</v>
       </c>
@@ -4905,10 +5026,12 @@
       <c r="K35" t="s">
         <v>175</v>
       </c>
-      <c r="N35">
-        <v>1</v>
-      </c>
-      <c r="O35" s="1">
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35" t="n">
+        <v>1</v>
+      </c>
+      <c r="O35" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P35" t="s">
@@ -4933,7 +5056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="36">
       <c r="A36" t="s">
         <v>317</v>
       </c>
@@ -4967,10 +5090,12 @@
       <c r="K36" t="s">
         <v>323</v>
       </c>
-      <c r="N36">
-        <v>1</v>
-      </c>
-      <c r="O36" s="1">
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36" t="n">
+        <v>1</v>
+      </c>
+      <c r="O36" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P36" t="s">
@@ -4995,7 +5120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="37">
       <c r="A37" t="s">
         <v>324</v>
       </c>
@@ -5029,10 +5154,12 @@
       <c r="K37" t="s">
         <v>328</v>
       </c>
-      <c r="N37">
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37" t="n">
         <v>0.71</v>
       </c>
-      <c r="O37" s="1">
+      <c r="O37" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P37" t="s">
@@ -5057,7 +5184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="38">
       <c r="A38" t="s">
         <v>329</v>
       </c>
@@ -5091,10 +5218,12 @@
       <c r="K38" t="s">
         <v>175</v>
       </c>
-      <c r="N38">
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38" t="n">
         <v>0.65</v>
       </c>
-      <c r="O38" s="1">
+      <c r="O38" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P38" t="s">
@@ -5119,7 +5248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="39">
       <c r="A39" t="s">
         <v>331</v>
       </c>
@@ -5153,10 +5282,12 @@
       <c r="K39" t="s">
         <v>175</v>
       </c>
-      <c r="N39">
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39" t="n">
         <v>0.99</v>
       </c>
-      <c r="O39" s="1">
+      <c r="O39" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P39" t="s">
@@ -5181,7 +5312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="40">
       <c r="A40" t="s">
         <v>334</v>
       </c>
@@ -5215,10 +5346,12 @@
       <c r="K40" t="s">
         <v>338</v>
       </c>
-      <c r="N40">
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40" t="n">
         <v>0.98</v>
       </c>
-      <c r="O40" s="1">
+      <c r="O40" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P40" t="s">
@@ -5243,7 +5376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="41">
       <c r="A41" t="s">
         <v>339</v>
       </c>
@@ -5277,10 +5410,12 @@
       <c r="K41" t="s">
         <v>345</v>
       </c>
-      <c r="N41">
-        <v>1</v>
-      </c>
-      <c r="O41" s="1">
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41" t="n">
+        <v>1</v>
+      </c>
+      <c r="O41" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P41" t="s">
@@ -5305,7 +5440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="42">
       <c r="A42" t="s">
         <v>346</v>
       </c>
@@ -5339,10 +5474,12 @@
       <c r="K42" t="s">
         <v>350</v>
       </c>
-      <c r="N42">
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42" t="n">
         <v>0.68</v>
       </c>
-      <c r="O42" s="1">
+      <c r="O42" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P42" t="s">
@@ -5367,7 +5504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="43">
       <c r="A43" t="s">
         <v>351</v>
       </c>
@@ -5401,10 +5538,12 @@
       <c r="K43" t="s">
         <v>175</v>
       </c>
-      <c r="N43">
-        <v>1</v>
-      </c>
-      <c r="O43" s="1">
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43" t="n">
+        <v>1</v>
+      </c>
+      <c r="O43" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P43" t="s">
@@ -5429,7 +5568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="44">
       <c r="A44" t="s">
         <v>353</v>
       </c>
@@ -5463,10 +5602,12 @@
       <c r="K44" t="s">
         <v>356</v>
       </c>
-      <c r="N44">
-        <v>1</v>
-      </c>
-      <c r="O44" s="1">
+      <c r="L44"/>
+      <c r="M44"/>
+      <c r="N44" t="n">
+        <v>1</v>
+      </c>
+      <c r="O44" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P44" t="s">
@@ -5491,7 +5632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="45">
       <c r="A45" t="s">
         <v>357</v>
       </c>
@@ -5525,10 +5666,12 @@
       <c r="K45" t="s">
         <v>175</v>
       </c>
-      <c r="N45">
-        <v>1</v>
-      </c>
-      <c r="O45" s="1">
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45" t="n">
+        <v>1</v>
+      </c>
+      <c r="O45" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P45" t="s">
@@ -5553,7 +5696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="46">
       <c r="A46" t="s">
         <v>359</v>
       </c>
@@ -5587,10 +5730,12 @@
       <c r="K46" t="s">
         <v>272</v>
       </c>
-      <c r="N46">
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46" t="n">
         <v>0.99</v>
       </c>
-      <c r="O46" s="1">
+      <c r="O46" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P46" t="s">
@@ -5615,7 +5760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="47">
       <c r="A47" t="s">
         <v>361</v>
       </c>
@@ -5649,10 +5794,12 @@
       <c r="K47" t="s">
         <v>175</v>
       </c>
-      <c r="N47">
-        <v>1</v>
-      </c>
-      <c r="O47" s="1">
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47" t="n">
+        <v>1</v>
+      </c>
+      <c r="O47" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P47" t="s">
@@ -5677,7 +5824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="48">
       <c r="A48" t="s">
         <v>363</v>
       </c>
@@ -5711,10 +5858,12 @@
       <c r="K48" t="s">
         <v>175</v>
       </c>
-      <c r="N48">
-        <v>1</v>
-      </c>
-      <c r="O48" s="1">
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48" t="n">
+        <v>1</v>
+      </c>
+      <c r="O48" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P48" t="s">
@@ -5739,7 +5888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="49">
       <c r="A49" t="s">
         <v>365</v>
       </c>
@@ -5773,10 +5922,12 @@
       <c r="K49" t="s">
         <v>370</v>
       </c>
-      <c r="N49">
+      <c r="L49"/>
+      <c r="M49"/>
+      <c r="N49" t="n">
         <v>0.54</v>
       </c>
-      <c r="O49" s="1">
+      <c r="O49" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P49" t="s">
@@ -5801,7 +5952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="50">
       <c r="A50" t="s">
         <v>371</v>
       </c>
@@ -5835,10 +5986,12 @@
       <c r="K50" t="s">
         <v>375</v>
       </c>
-      <c r="N50">
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50" t="n">
         <v>0.61</v>
       </c>
-      <c r="O50" s="1">
+      <c r="O50" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P50" t="s">
@@ -5863,7 +6016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="51">
       <c r="A51" t="s">
         <v>376</v>
       </c>
@@ -5897,10 +6050,12 @@
       <c r="K51" t="s">
         <v>175</v>
       </c>
-      <c r="N51">
-        <v>1</v>
-      </c>
-      <c r="O51" s="1">
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="N51" t="n">
+        <v>1</v>
+      </c>
+      <c r="O51" s="1" t="n">
         <v>45104</v>
       </c>
       <c r="P51" t="s">
@@ -5927,6 +6082,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>